<commit_message>
Actualización automática: 2025-03-05 15:25:49
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\8\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp16499\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06FD4C4-9949-486B-AFED-2506814E6A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24625DB-4347-42EC-98C5-3854AA9F0ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="151">
   <si>
     <t>Host</t>
   </si>
@@ -469,6 +469,15 @@
   </si>
   <si>
     <t>SOC</t>
+  </si>
+  <si>
+    <t>10.181.11.192</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>crmtestmicros</t>
   </si>
 </sst>
 </file>
@@ -817,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E68"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,6 +2021,23 @@
         <v>146</v>
       </c>
     </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-11 15:25:32
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp16499\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp24419\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24625DB-4347-42EC-98C5-3854AA9F0ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E65737-5093-42A8-90BC-3DF003673E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1794,7 @@
         <v>119</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-13 14:50:41
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp24419\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\10\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E65737-5093-42A8-90BC-3DF003673E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A373DCCE-70F7-450C-9587-EC4A6891FB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="152">
   <si>
     <t>Host</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>crmtestmicros</t>
+  </si>
+  <si>
+    <t>LOTE11-General</t>
   </si>
 </sst>
 </file>
@@ -828,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,7 +1655,7 @@
         <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>103</v>
@@ -1737,7 +1740,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>113</v>
@@ -1805,7 +1808,7 @@
         <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>121</v>
@@ -1822,7 +1825,7 @@
         <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>123</v>
@@ -1839,7 +1842,7 @@
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>125</v>
@@ -1856,7 +1859,7 @@
         <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>127</v>
@@ -1873,7 +1876,7 @@
         <v>129</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>129</v>
@@ -1890,7 +1893,7 @@
         <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>131</v>
@@ -1907,7 +1910,7 @@
         <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>133</v>
@@ -1924,7 +1927,7 @@
         <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>135</v>
@@ -1941,7 +1944,7 @@
         <v>137</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>137</v>
@@ -1958,7 +1961,7 @@
         <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 14:03:44
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\10\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp02844\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A373DCCE-70F7-450C-9587-EC4A6891FB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5927E9-5D1B-4CB6-AFF7-261E7BAB064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>10.181.11.135</t>
   </si>
   <si>
-    <t>moviltrack_db_desanew</t>
-  </si>
-  <si>
     <t>10.181.11.134</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>LOTE11-General</t>
+  </si>
+  <si>
+    <t>plantillaOL9</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1655,7 @@
         <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>103</v>
@@ -1740,7 +1740,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>113</v>
@@ -1783,262 +1783,262 @@
         <v>7</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
         <v>99</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B56" t="s">
-        <v>151</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B57" t="s">
-        <v>151</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>151</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B59" t="s">
-        <v>151</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B60" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="B61" t="s">
-        <v>151</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B62" t="s">
-        <v>151</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="B63" t="s">
-        <v>151</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D64" t="s">
         <v>97</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
         <v>97</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D66" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
         <v>148</v>
       </c>
-      <c r="B69" t="s">
-        <v>149</v>
-      </c>
       <c r="C69" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D69" t="s">
         <v>97</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 14:24:10
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp02844\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp21787\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5927E9-5D1B-4CB6-AFF7-261E7BAB064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C0A51D-BB54-48A6-B379-A858A78E8D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
   <si>
     <t>Host</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>plantillaOL9</t>
+  </si>
+  <si>
+    <t>10.181.8.226</t>
+  </si>
+  <si>
+    <t>Goldengate</t>
+  </si>
+  <si>
+    <t>goldengateapp</t>
   </si>
 </sst>
 </file>
@@ -829,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,6 +2050,23 @@
         <v>149</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 16:54:45
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp21787\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C0A51D-BB54-48A6-B379-A858A78E8D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF76400-EE95-4681-9464-AFF6FF45C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
   <si>
     <t>Host</t>
   </si>
@@ -490,6 +490,363 @@
   </si>
   <si>
     <t>goldengateapp</t>
+  </si>
+  <si>
+    <t>10.112.3.4</t>
+  </si>
+  <si>
+    <t>10.139.2.3</t>
+  </si>
+  <si>
+    <t>10.134.3.4</t>
+  </si>
+  <si>
+    <t>10.187.3.4</t>
+  </si>
+  <si>
+    <t>10.189.3.4</t>
+  </si>
+  <si>
+    <t>10.34.3.3</t>
+  </si>
+  <si>
+    <t>10.65.3.4</t>
+  </si>
+  <si>
+    <t>10.190.3.4</t>
+  </si>
+  <si>
+    <t>10.231.3.4</t>
+  </si>
+  <si>
+    <t>10.92.3.4</t>
+  </si>
+  <si>
+    <t>172.16.4.4</t>
+  </si>
+  <si>
+    <t>10.115.3.4</t>
+  </si>
+  <si>
+    <t>10.91.3.7</t>
+  </si>
+  <si>
+    <t>10.147.3.5</t>
+  </si>
+  <si>
+    <t>10.127.0.7</t>
+  </si>
+  <si>
+    <t>10.203.3.4</t>
+  </si>
+  <si>
+    <t>172.16.6.8</t>
+  </si>
+  <si>
+    <t>172.16.8.3</t>
+  </si>
+  <si>
+    <t>172.16.9.3</t>
+  </si>
+  <si>
+    <t>172.16.10.6</t>
+  </si>
+  <si>
+    <t>10.156.3.7</t>
+  </si>
+  <si>
+    <t>10.155.3.4</t>
+  </si>
+  <si>
+    <t>10.144.3.7</t>
+  </si>
+  <si>
+    <t>10.149.3.7</t>
+  </si>
+  <si>
+    <t>10.29.3.5</t>
+  </si>
+  <si>
+    <t>10.86.0.16</t>
+  </si>
+  <si>
+    <t>10.87.3.8</t>
+  </si>
+  <si>
+    <t>10.108.3.87</t>
+  </si>
+  <si>
+    <t>10.49.3.8</t>
+  </si>
+  <si>
+    <t>10.71.3.5</t>
+  </si>
+  <si>
+    <t>10.32.3.8</t>
+  </si>
+  <si>
+    <t>10.109.3.8</t>
+  </si>
+  <si>
+    <t>10.104.3.3</t>
+  </si>
+  <si>
+    <t>10.122.3.3</t>
+  </si>
+  <si>
+    <t>10.129.3.5</t>
+  </si>
+  <si>
+    <t>10.46.3.8</t>
+  </si>
+  <si>
+    <t>10.48.3.8</t>
+  </si>
+  <si>
+    <t>10.145.3.7</t>
+  </si>
+  <si>
+    <t>10.151.3.3</t>
+  </si>
+  <si>
+    <t>10.89.3.3</t>
+  </si>
+  <si>
+    <t>10.232.3.6</t>
+  </si>
+  <si>
+    <t>172.16.7.15</t>
+  </si>
+  <si>
+    <t>172.16.90.3</t>
+  </si>
+  <si>
+    <t>172.16.91.7</t>
+  </si>
+  <si>
+    <t>172.16.11.7</t>
+  </si>
+  <si>
+    <t>172.16.3.6</t>
+  </si>
+  <si>
+    <t>172.16.107.7</t>
+  </si>
+  <si>
+    <t>172.16.116.80</t>
+  </si>
+  <si>
+    <t>10.16.77.4</t>
+  </si>
+  <si>
+    <t>10.173.3.7</t>
+  </si>
+  <si>
+    <t>10.121.0.6</t>
+  </si>
+  <si>
+    <t>172.16.134.4</t>
+  </si>
+  <si>
+    <t>10.125.3.8</t>
+  </si>
+  <si>
+    <t>10.245.3.4</t>
+  </si>
+  <si>
+    <t>ansible_test</t>
+  </si>
+  <si>
+    <t>Srv_Geo_Bk</t>
+  </si>
+  <si>
+    <t>alper-n1</t>
+  </si>
+  <si>
+    <t>alct2-bk</t>
+  </si>
+  <si>
+    <t>alflo-n1</t>
+  </si>
+  <si>
+    <t>alca5-n1</t>
+  </si>
+  <si>
+    <t>alarm-n1</t>
+  </si>
+  <si>
+    <t>alave-n1</t>
+  </si>
+  <si>
+    <t>ktman-n1</t>
+  </si>
+  <si>
+    <t>ktark-n1</t>
+  </si>
+  <si>
+    <t>ktgir-n1</t>
+  </si>
+  <si>
+    <t>ktpob-bk</t>
+  </si>
+  <si>
+    <t>akven-n1</t>
+  </si>
+  <si>
+    <t>kttes-bk</t>
+  </si>
+  <si>
+    <t>ktsal-n2</t>
+  </si>
+  <si>
+    <t>ktuno-n1</t>
+  </si>
+  <si>
+    <t>ktjul-n1</t>
+  </si>
+  <si>
+    <t>ktfus-n1</t>
+  </si>
+  <si>
+    <t>akbol-bk</t>
+  </si>
+  <si>
+    <t>akipi-bk</t>
+  </si>
+  <si>
+    <t>akper-n1</t>
+  </si>
+  <si>
+    <t>ak170-n1</t>
+  </si>
+  <si>
+    <t>alva2-new</t>
+  </si>
+  <si>
+    <t>alpie-n1</t>
+  </si>
+  <si>
+    <t>aliba-bk</t>
+  </si>
+  <si>
+    <t>alnei-bk</t>
+  </si>
+  <si>
+    <t>almol-n2</t>
+  </si>
+  <si>
+    <t>alkun-n2</t>
+  </si>
+  <si>
+    <t>almay-bk</t>
+  </si>
+  <si>
+    <t>albel-new</t>
+  </si>
+  <si>
+    <t>alnue-bk</t>
+  </si>
+  <si>
+    <t>ktb94-n1</t>
+  </si>
+  <si>
+    <t>ktchi-bk</t>
+  </si>
+  <si>
+    <t>ktame-bk</t>
+  </si>
+  <si>
+    <t>ktmay-n1</t>
+  </si>
+  <si>
+    <t>kttit-bk</t>
+  </si>
+  <si>
+    <t>ktbuc-bk</t>
+  </si>
+  <si>
+    <t>ktsoa-bk</t>
+  </si>
+  <si>
+    <t>ktcal-bk</t>
+  </si>
+  <si>
+    <t>ktmos-bk</t>
+  </si>
+  <si>
+    <t>ktvil-bk</t>
+  </si>
+  <si>
+    <t>ktsba-n1</t>
+  </si>
+  <si>
+    <t>ktbar-n1</t>
+  </si>
+  <si>
+    <t>akpas-bk</t>
+  </si>
+  <si>
+    <t>aktuq-n1</t>
+  </si>
+  <si>
+    <t>akigp-bk</t>
+  </si>
+  <si>
+    <t>akb30-n1</t>
+  </si>
+  <si>
+    <t>akb68-n1</t>
+  </si>
+  <si>
+    <t>akvil-n1</t>
+  </si>
+  <si>
+    <t>akbar-bk</t>
+  </si>
+  <si>
+    <t>aksin-bk</t>
+  </si>
+  <si>
+    <t>akcan-n1</t>
+  </si>
+  <si>
+    <t>alapa-bk</t>
+  </si>
+  <si>
+    <t>akyop-n1</t>
+  </si>
+  <si>
+    <t>akede-n1</t>
+  </si>
+  <si>
+    <t>albu2-bk</t>
+  </si>
+  <si>
+    <t>ktnqs-n1</t>
+  </si>
+  <si>
+    <t>alba5-bk</t>
+  </si>
+  <si>
+    <t>albuc-n1</t>
+  </si>
+  <si>
+    <t>alrio-n1</t>
+  </si>
+  <si>
+    <t>aldie-n1</t>
+  </si>
+  <si>
+    <t>10.45.3.7</t>
+  </si>
+  <si>
+    <t>10.178.3.4</t>
+  </si>
+  <si>
+    <t>10.98.3.4</t>
+  </si>
+  <si>
+    <t>10.106.3.4</t>
   </si>
 </sst>
 </file>
@@ -545,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2427,1009 @@
         <v>154</v>
       </c>
     </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D71" t="s">
+        <v>209</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D72" t="s">
+        <v>209</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D73" t="s">
+        <v>209</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D74" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
+        <v>209</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" t="s">
+        <v>209</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" t="s">
+        <v>209</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" t="s">
+        <v>209</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" t="s">
+        <v>209</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D82" t="s">
+        <v>209</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83" t="s">
+        <v>209</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D84" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" t="s">
+        <v>209</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D87" t="s">
+        <v>209</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D89" t="s">
+        <v>209</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D90" t="s">
+        <v>209</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D92" t="s">
+        <v>209</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D94" t="s">
+        <v>209</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D95" t="s">
+        <v>209</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D96" t="s">
+        <v>209</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D97" t="s">
+        <v>209</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D98" t="s">
+        <v>209</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D99" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D100" t="s">
+        <v>209</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D101" t="s">
+        <v>209</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D102" t="s">
+        <v>209</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D103" t="s">
+        <v>209</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D104" t="s">
+        <v>209</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D105" t="s">
+        <v>209</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D106" t="s">
+        <v>209</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D107" t="s">
+        <v>209</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D108" t="s">
+        <v>209</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D109" t="s">
+        <v>209</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D110" t="s">
+        <v>209</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D111" t="s">
+        <v>209</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D112" t="s">
+        <v>209</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D113" t="s">
+        <v>209</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D114" t="s">
+        <v>209</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D115" t="s">
+        <v>209</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D116" t="s">
+        <v>209</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D117" t="s">
+        <v>209</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" t="s">
+        <v>209</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="D119" t="s">
+        <v>209</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D120" t="s">
+        <v>209</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D121" t="s">
+        <v>209</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D122" t="s">
+        <v>209</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D123" t="s">
+        <v>209</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D124" t="s">
+        <v>209</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D125" t="s">
+        <v>209</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D126" t="s">
+        <v>209</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D127" t="s">
+        <v>209</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D128" t="s">
+        <v>209</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D129" t="s">
+        <v>209</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 16:57:30
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF76400-EE95-4681-9464-AFF6FF45C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B63653-799C-4C3F-89EB-431E75068D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,9 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,13 +3241,13 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="6">
+      <c r="A119" s="5">
         <v>147127110112</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C119" s="6">
+      <c r="C119" s="5">
         <v>147127110112</v>
       </c>
       <c r="D119" t="s">

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:02:54
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B63653-799C-4C3F-89EB-431E75068D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C30158E-CE70-433B-AB94-EBFFAAAB10E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
   <si>
     <t>Host</t>
   </si>
@@ -490,363 +490,6 @@
   </si>
   <si>
     <t>goldengateapp</t>
-  </si>
-  <si>
-    <t>10.112.3.4</t>
-  </si>
-  <si>
-    <t>10.139.2.3</t>
-  </si>
-  <si>
-    <t>10.134.3.4</t>
-  </si>
-  <si>
-    <t>10.187.3.4</t>
-  </si>
-  <si>
-    <t>10.189.3.4</t>
-  </si>
-  <si>
-    <t>10.34.3.3</t>
-  </si>
-  <si>
-    <t>10.65.3.4</t>
-  </si>
-  <si>
-    <t>10.190.3.4</t>
-  </si>
-  <si>
-    <t>10.231.3.4</t>
-  </si>
-  <si>
-    <t>10.92.3.4</t>
-  </si>
-  <si>
-    <t>172.16.4.4</t>
-  </si>
-  <si>
-    <t>10.115.3.4</t>
-  </si>
-  <si>
-    <t>10.91.3.7</t>
-  </si>
-  <si>
-    <t>10.147.3.5</t>
-  </si>
-  <si>
-    <t>10.127.0.7</t>
-  </si>
-  <si>
-    <t>10.203.3.4</t>
-  </si>
-  <si>
-    <t>172.16.6.8</t>
-  </si>
-  <si>
-    <t>172.16.8.3</t>
-  </si>
-  <si>
-    <t>172.16.9.3</t>
-  </si>
-  <si>
-    <t>172.16.10.6</t>
-  </si>
-  <si>
-    <t>10.156.3.7</t>
-  </si>
-  <si>
-    <t>10.155.3.4</t>
-  </si>
-  <si>
-    <t>10.144.3.7</t>
-  </si>
-  <si>
-    <t>10.149.3.7</t>
-  </si>
-  <si>
-    <t>10.29.3.5</t>
-  </si>
-  <si>
-    <t>10.86.0.16</t>
-  </si>
-  <si>
-    <t>10.87.3.8</t>
-  </si>
-  <si>
-    <t>10.108.3.87</t>
-  </si>
-  <si>
-    <t>10.49.3.8</t>
-  </si>
-  <si>
-    <t>10.71.3.5</t>
-  </si>
-  <si>
-    <t>10.32.3.8</t>
-  </si>
-  <si>
-    <t>10.109.3.8</t>
-  </si>
-  <si>
-    <t>10.104.3.3</t>
-  </si>
-  <si>
-    <t>10.122.3.3</t>
-  </si>
-  <si>
-    <t>10.129.3.5</t>
-  </si>
-  <si>
-    <t>10.46.3.8</t>
-  </si>
-  <si>
-    <t>10.48.3.8</t>
-  </si>
-  <si>
-    <t>10.145.3.7</t>
-  </si>
-  <si>
-    <t>10.151.3.3</t>
-  </si>
-  <si>
-    <t>10.89.3.3</t>
-  </si>
-  <si>
-    <t>10.232.3.6</t>
-  </si>
-  <si>
-    <t>172.16.7.15</t>
-  </si>
-  <si>
-    <t>172.16.90.3</t>
-  </si>
-  <si>
-    <t>172.16.91.7</t>
-  </si>
-  <si>
-    <t>172.16.11.7</t>
-  </si>
-  <si>
-    <t>172.16.3.6</t>
-  </si>
-  <si>
-    <t>172.16.107.7</t>
-  </si>
-  <si>
-    <t>172.16.116.80</t>
-  </si>
-  <si>
-    <t>10.16.77.4</t>
-  </si>
-  <si>
-    <t>10.173.3.7</t>
-  </si>
-  <si>
-    <t>10.121.0.6</t>
-  </si>
-  <si>
-    <t>172.16.134.4</t>
-  </si>
-  <si>
-    <t>10.125.3.8</t>
-  </si>
-  <si>
-    <t>10.245.3.4</t>
-  </si>
-  <si>
-    <t>ansible_test</t>
-  </si>
-  <si>
-    <t>Srv_Geo_Bk</t>
-  </si>
-  <si>
-    <t>alper-n1</t>
-  </si>
-  <si>
-    <t>alct2-bk</t>
-  </si>
-  <si>
-    <t>alflo-n1</t>
-  </si>
-  <si>
-    <t>alca5-n1</t>
-  </si>
-  <si>
-    <t>alarm-n1</t>
-  </si>
-  <si>
-    <t>alave-n1</t>
-  </si>
-  <si>
-    <t>ktman-n1</t>
-  </si>
-  <si>
-    <t>ktark-n1</t>
-  </si>
-  <si>
-    <t>ktgir-n1</t>
-  </si>
-  <si>
-    <t>ktpob-bk</t>
-  </si>
-  <si>
-    <t>akven-n1</t>
-  </si>
-  <si>
-    <t>kttes-bk</t>
-  </si>
-  <si>
-    <t>ktsal-n2</t>
-  </si>
-  <si>
-    <t>ktuno-n1</t>
-  </si>
-  <si>
-    <t>ktjul-n1</t>
-  </si>
-  <si>
-    <t>ktfus-n1</t>
-  </si>
-  <si>
-    <t>akbol-bk</t>
-  </si>
-  <si>
-    <t>akipi-bk</t>
-  </si>
-  <si>
-    <t>akper-n1</t>
-  </si>
-  <si>
-    <t>ak170-n1</t>
-  </si>
-  <si>
-    <t>alva2-new</t>
-  </si>
-  <si>
-    <t>alpie-n1</t>
-  </si>
-  <si>
-    <t>aliba-bk</t>
-  </si>
-  <si>
-    <t>alnei-bk</t>
-  </si>
-  <si>
-    <t>almol-n2</t>
-  </si>
-  <si>
-    <t>alkun-n2</t>
-  </si>
-  <si>
-    <t>almay-bk</t>
-  </si>
-  <si>
-    <t>albel-new</t>
-  </si>
-  <si>
-    <t>alnue-bk</t>
-  </si>
-  <si>
-    <t>ktb94-n1</t>
-  </si>
-  <si>
-    <t>ktchi-bk</t>
-  </si>
-  <si>
-    <t>ktame-bk</t>
-  </si>
-  <si>
-    <t>ktmay-n1</t>
-  </si>
-  <si>
-    <t>kttit-bk</t>
-  </si>
-  <si>
-    <t>ktbuc-bk</t>
-  </si>
-  <si>
-    <t>ktsoa-bk</t>
-  </si>
-  <si>
-    <t>ktcal-bk</t>
-  </si>
-  <si>
-    <t>ktmos-bk</t>
-  </si>
-  <si>
-    <t>ktvil-bk</t>
-  </si>
-  <si>
-    <t>ktsba-n1</t>
-  </si>
-  <si>
-    <t>ktbar-n1</t>
-  </si>
-  <si>
-    <t>akpas-bk</t>
-  </si>
-  <si>
-    <t>aktuq-n1</t>
-  </si>
-  <si>
-    <t>akigp-bk</t>
-  </si>
-  <si>
-    <t>akb30-n1</t>
-  </si>
-  <si>
-    <t>akb68-n1</t>
-  </si>
-  <si>
-    <t>akvil-n1</t>
-  </si>
-  <si>
-    <t>akbar-bk</t>
-  </si>
-  <si>
-    <t>aksin-bk</t>
-  </si>
-  <si>
-    <t>akcan-n1</t>
-  </si>
-  <si>
-    <t>alapa-bk</t>
-  </si>
-  <si>
-    <t>akyop-n1</t>
-  </si>
-  <si>
-    <t>akede-n1</t>
-  </si>
-  <si>
-    <t>albu2-bk</t>
-  </si>
-  <si>
-    <t>ktnqs-n1</t>
-  </si>
-  <si>
-    <t>alba5-bk</t>
-  </si>
-  <si>
-    <t>albuc-n1</t>
-  </si>
-  <si>
-    <t>alrio-n1</t>
-  </si>
-  <si>
-    <t>aldie-n1</t>
-  </si>
-  <si>
-    <t>10.45.3.7</t>
-  </si>
-  <si>
-    <t>10.178.3.4</t>
-  </si>
-  <si>
-    <t>10.98.3.4</t>
-  </si>
-  <si>
-    <t>10.106.3.4</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,1009 +2067,6 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D71" t="s">
-        <v>209</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="D72" t="s">
-        <v>209</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="D73" t="s">
-        <v>209</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D74" t="s">
-        <v>209</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D75" t="s">
-        <v>209</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D76" t="s">
-        <v>209</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" t="s">
-        <v>209</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D78" t="s">
-        <v>209</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D79" t="s">
-        <v>209</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D80" t="s">
-        <v>209</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" t="s">
-        <v>209</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D82" t="s">
-        <v>209</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D83" t="s">
-        <v>209</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D84" t="s">
-        <v>209</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D85" t="s">
-        <v>209</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D86" t="s">
-        <v>209</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D87" t="s">
-        <v>209</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D88" t="s">
-        <v>209</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D89" t="s">
-        <v>209</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D90" t="s">
-        <v>209</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D91" t="s">
-        <v>209</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D92" t="s">
-        <v>209</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D93" t="s">
-        <v>209</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D94" t="s">
-        <v>209</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D95" t="s">
-        <v>209</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D96" t="s">
-        <v>209</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D97" t="s">
-        <v>209</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D98" t="s">
-        <v>209</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D99" t="s">
-        <v>209</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D100" t="s">
-        <v>209</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D101" t="s">
-        <v>209</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D102" t="s">
-        <v>209</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D103" t="s">
-        <v>209</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D104" t="s">
-        <v>209</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D105" t="s">
-        <v>209</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D106" t="s">
-        <v>209</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D107" t="s">
-        <v>209</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D108" t="s">
-        <v>209</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D109" t="s">
-        <v>209</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D110" t="s">
-        <v>209</v>
-      </c>
-      <c r="E110" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D111" t="s">
-        <v>209</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D112" t="s">
-        <v>209</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D113" t="s">
-        <v>209</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D114" t="s">
-        <v>209</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D115" t="s">
-        <v>209</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D116" t="s">
-        <v>209</v>
-      </c>
-      <c r="E116" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D117" t="s">
-        <v>209</v>
-      </c>
-      <c r="E117" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D118" t="s">
-        <v>209</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="5">
-        <v>147127110112</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C119" s="5">
-        <v>147127110112</v>
-      </c>
-      <c r="D119" t="s">
-        <v>209</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C120" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D120" t="s">
-        <v>209</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D121" t="s">
-        <v>209</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D122" t="s">
-        <v>209</v>
-      </c>
-      <c r="E122" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D123" t="s">
-        <v>209</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D124" t="s">
-        <v>209</v>
-      </c>
-      <c r="E124" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D125" t="s">
-        <v>209</v>
-      </c>
-      <c r="E125" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D126" t="s">
-        <v>209</v>
-      </c>
-      <c r="E126" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D127" t="s">
-        <v>209</v>
-      </c>
-      <c r="E127" s="5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C128" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D128" t="s">
-        <v>209</v>
-      </c>
-      <c r="E128" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D129" t="s">
-        <v>209</v>
-      </c>
-      <c r="E129" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:04:53
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C30158E-CE70-433B-AB94-EBFFAAAB10E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAEFDA-893A-4645-9F8C-D1DC74889EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
   <si>
     <t>Host</t>
   </si>
@@ -490,6 +490,363 @@
   </si>
   <si>
     <t>goldengateapp</t>
+  </si>
+  <si>
+    <t>10.112.3.4</t>
+  </si>
+  <si>
+    <t>10.139.2.3</t>
+  </si>
+  <si>
+    <t>10.134.3.4</t>
+  </si>
+  <si>
+    <t>10.187.3.4</t>
+  </si>
+  <si>
+    <t>10.189.3.4</t>
+  </si>
+  <si>
+    <t>10.34.3.3</t>
+  </si>
+  <si>
+    <t>10.65.3.4</t>
+  </si>
+  <si>
+    <t>10.190.3.4</t>
+  </si>
+  <si>
+    <t>10.231.3.4</t>
+  </si>
+  <si>
+    <t>10.92.3.4</t>
+  </si>
+  <si>
+    <t>172.16.4.4</t>
+  </si>
+  <si>
+    <t>10.115.3.4</t>
+  </si>
+  <si>
+    <t>10.91.3.7</t>
+  </si>
+  <si>
+    <t>10.147.3.5</t>
+  </si>
+  <si>
+    <t>10.127.0.7</t>
+  </si>
+  <si>
+    <t>10.203.3.4</t>
+  </si>
+  <si>
+    <t>172.16.6.8</t>
+  </si>
+  <si>
+    <t>172.16.8.3</t>
+  </si>
+  <si>
+    <t>172.16.9.3</t>
+  </si>
+  <si>
+    <t>172.16.10.6</t>
+  </si>
+  <si>
+    <t>10.156.3.7</t>
+  </si>
+  <si>
+    <t>10.155.3.4</t>
+  </si>
+  <si>
+    <t>10.144.3.7</t>
+  </si>
+  <si>
+    <t>10.149.3.7</t>
+  </si>
+  <si>
+    <t>10.29.3.5</t>
+  </si>
+  <si>
+    <t>10.86.0.16</t>
+  </si>
+  <si>
+    <t>10.87.3.8</t>
+  </si>
+  <si>
+    <t>10.108.3.87</t>
+  </si>
+  <si>
+    <t>10.49.3.8</t>
+  </si>
+  <si>
+    <t>10.71.3.5</t>
+  </si>
+  <si>
+    <t>10.32.3.8</t>
+  </si>
+  <si>
+    <t>10.109.3.8</t>
+  </si>
+  <si>
+    <t>10.104.3.3</t>
+  </si>
+  <si>
+    <t>10.122.3.3</t>
+  </si>
+  <si>
+    <t>10.129.3.5</t>
+  </si>
+  <si>
+    <t>10.46.3.8</t>
+  </si>
+  <si>
+    <t>10.48.3.8</t>
+  </si>
+  <si>
+    <t>10.145.3.7</t>
+  </si>
+  <si>
+    <t>10.151.3.3</t>
+  </si>
+  <si>
+    <t>10.89.3.3</t>
+  </si>
+  <si>
+    <t>10.232.3.6</t>
+  </si>
+  <si>
+    <t>172.16.7.15</t>
+  </si>
+  <si>
+    <t>172.16.90.3</t>
+  </si>
+  <si>
+    <t>172.16.91.7</t>
+  </si>
+  <si>
+    <t>172.16.11.7</t>
+  </si>
+  <si>
+    <t>172.16.3.6</t>
+  </si>
+  <si>
+    <t>172.16.107.7</t>
+  </si>
+  <si>
+    <t>172.16.116.80</t>
+  </si>
+  <si>
+    <t>10.16.77.4</t>
+  </si>
+  <si>
+    <t>10.173.3.7</t>
+  </si>
+  <si>
+    <t>10.121.0.6</t>
+  </si>
+  <si>
+    <t>172.16.134.4</t>
+  </si>
+  <si>
+    <t>10.125.3.8</t>
+  </si>
+  <si>
+    <t>10.245.3.4</t>
+  </si>
+  <si>
+    <t>ansible_test</t>
+  </si>
+  <si>
+    <t>Srv_Geo_Bk</t>
+  </si>
+  <si>
+    <t>alper-n1</t>
+  </si>
+  <si>
+    <t>alct2-bk</t>
+  </si>
+  <si>
+    <t>alflo-n1</t>
+  </si>
+  <si>
+    <t>alca5-n1</t>
+  </si>
+  <si>
+    <t>alarm-n1</t>
+  </si>
+  <si>
+    <t>alave-n1</t>
+  </si>
+  <si>
+    <t>ktman-n1</t>
+  </si>
+  <si>
+    <t>ktark-n1</t>
+  </si>
+  <si>
+    <t>ktgir-n1</t>
+  </si>
+  <si>
+    <t>ktpob-bk</t>
+  </si>
+  <si>
+    <t>akven-n1</t>
+  </si>
+  <si>
+    <t>kttes-bk</t>
+  </si>
+  <si>
+    <t>ktsal-n2</t>
+  </si>
+  <si>
+    <t>ktuno-n1</t>
+  </si>
+  <si>
+    <t>ktjul-n1</t>
+  </si>
+  <si>
+    <t>ktfus-n1</t>
+  </si>
+  <si>
+    <t>akbol-bk</t>
+  </si>
+  <si>
+    <t>akipi-bk</t>
+  </si>
+  <si>
+    <t>akper-n1</t>
+  </si>
+  <si>
+    <t>ak170-n1</t>
+  </si>
+  <si>
+    <t>alva2-new</t>
+  </si>
+  <si>
+    <t>alpie-n1</t>
+  </si>
+  <si>
+    <t>aliba-bk</t>
+  </si>
+  <si>
+    <t>alnei-bk</t>
+  </si>
+  <si>
+    <t>almol-n2</t>
+  </si>
+  <si>
+    <t>alkun-n2</t>
+  </si>
+  <si>
+    <t>almay-bk</t>
+  </si>
+  <si>
+    <t>albel-new</t>
+  </si>
+  <si>
+    <t>alnue-bk</t>
+  </si>
+  <si>
+    <t>ktb94-n1</t>
+  </si>
+  <si>
+    <t>ktchi-bk</t>
+  </si>
+  <si>
+    <t>ktame-bk</t>
+  </si>
+  <si>
+    <t>ktmay-n1</t>
+  </si>
+  <si>
+    <t>kttit-bk</t>
+  </si>
+  <si>
+    <t>ktbuc-bk</t>
+  </si>
+  <si>
+    <t>ktsoa-bk</t>
+  </si>
+  <si>
+    <t>ktcal-bk</t>
+  </si>
+  <si>
+    <t>ktmos-bk</t>
+  </si>
+  <si>
+    <t>ktvil-bk</t>
+  </si>
+  <si>
+    <t>ktsba-n1</t>
+  </si>
+  <si>
+    <t>ktbar-n1</t>
+  </si>
+  <si>
+    <t>akpas-bk</t>
+  </si>
+  <si>
+    <t>aktuq-n1</t>
+  </si>
+  <si>
+    <t>akigp-bk</t>
+  </si>
+  <si>
+    <t>akb30-n1</t>
+  </si>
+  <si>
+    <t>akb68-n1</t>
+  </si>
+  <si>
+    <t>akvil-n1</t>
+  </si>
+  <si>
+    <t>akbar-bk</t>
+  </si>
+  <si>
+    <t>aksin-bk</t>
+  </si>
+  <si>
+    <t>akcan-n1</t>
+  </si>
+  <si>
+    <t>alapa-bk</t>
+  </si>
+  <si>
+    <t>akyop-n1</t>
+  </si>
+  <si>
+    <t>akede-n1</t>
+  </si>
+  <si>
+    <t>albu2-bk</t>
+  </si>
+  <si>
+    <t>ktnqs-n1</t>
+  </si>
+  <si>
+    <t>alba5-bk</t>
+  </si>
+  <si>
+    <t>albuc-n1</t>
+  </si>
+  <si>
+    <t>alrio-n1</t>
+  </si>
+  <si>
+    <t>aldie-n1</t>
+  </si>
+  <si>
+    <t>10.45.3.7</t>
+  </si>
+  <si>
+    <t>10.178.3.4</t>
+  </si>
+  <si>
+    <t>10.98.3.4</t>
+  </si>
+  <si>
+    <t>10.106.3.4</t>
   </si>
 </sst>
 </file>
@@ -545,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2427,1009 @@
         <v>154</v>
       </c>
     </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>270</v>
+      </c>
+      <c r="B71" t="s">
+        <v>210</v>
+      </c>
+      <c r="C71" t="s">
+        <v>270</v>
+      </c>
+      <c r="D71" t="s">
+        <v>209</v>
+      </c>
+      <c r="E71" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>271</v>
+      </c>
+      <c r="B72" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" t="s">
+        <v>271</v>
+      </c>
+      <c r="D72" t="s">
+        <v>209</v>
+      </c>
+      <c r="E72" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" t="s">
+        <v>210</v>
+      </c>
+      <c r="C73" t="s">
+        <v>272</v>
+      </c>
+      <c r="D73" t="s">
+        <v>209</v>
+      </c>
+      <c r="E73" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>273</v>
+      </c>
+      <c r="B74" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" t="s">
+        <v>273</v>
+      </c>
+      <c r="D74" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
+        <v>209</v>
+      </c>
+      <c r="E76" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" t="s">
+        <v>209</v>
+      </c>
+      <c r="E77" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" t="s">
+        <v>209</v>
+      </c>
+      <c r="E78" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" t="s">
+        <v>209</v>
+      </c>
+      <c r="E79" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" t="s">
+        <v>210</v>
+      </c>
+      <c r="C80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" t="s">
+        <v>209</v>
+      </c>
+      <c r="E80" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" t="s">
+        <v>210</v>
+      </c>
+      <c r="C81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>210</v>
+      </c>
+      <c r="C82" t="s">
+        <v>162</v>
+      </c>
+      <c r="D82" t="s">
+        <v>209</v>
+      </c>
+      <c r="E82" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" t="s">
+        <v>210</v>
+      </c>
+      <c r="C83" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83" t="s">
+        <v>209</v>
+      </c>
+      <c r="E83" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" t="s">
+        <v>210</v>
+      </c>
+      <c r="C84" t="s">
+        <v>164</v>
+      </c>
+      <c r="D84" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>165</v>
+      </c>
+      <c r="B85" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" t="s">
+        <v>209</v>
+      </c>
+      <c r="E85" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" t="s">
+        <v>210</v>
+      </c>
+      <c r="C86" t="s">
+        <v>166</v>
+      </c>
+      <c r="D86" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" t="s">
+        <v>167</v>
+      </c>
+      <c r="D87" t="s">
+        <v>209</v>
+      </c>
+      <c r="E87" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" t="s">
+        <v>210</v>
+      </c>
+      <c r="C88" t="s">
+        <v>168</v>
+      </c>
+      <c r="D88" t="s">
+        <v>209</v>
+      </c>
+      <c r="E88" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B89" t="s">
+        <v>210</v>
+      </c>
+      <c r="C89" t="s">
+        <v>169</v>
+      </c>
+      <c r="D89" t="s">
+        <v>209</v>
+      </c>
+      <c r="E89" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" t="s">
+        <v>210</v>
+      </c>
+      <c r="C90" t="s">
+        <v>170</v>
+      </c>
+      <c r="D90" t="s">
+        <v>209</v>
+      </c>
+      <c r="E90" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91" t="s">
+        <v>210</v>
+      </c>
+      <c r="C91" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E91" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>172</v>
+      </c>
+      <c r="B92" t="s">
+        <v>210</v>
+      </c>
+      <c r="C92" t="s">
+        <v>172</v>
+      </c>
+      <c r="D92" t="s">
+        <v>209</v>
+      </c>
+      <c r="E92" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>173</v>
+      </c>
+      <c r="B93" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" t="s">
+        <v>173</v>
+      </c>
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+      <c r="E93" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" t="s">
+        <v>174</v>
+      </c>
+      <c r="D94" t="s">
+        <v>209</v>
+      </c>
+      <c r="E94" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" t="s">
+        <v>210</v>
+      </c>
+      <c r="C95" t="s">
+        <v>175</v>
+      </c>
+      <c r="D95" t="s">
+        <v>209</v>
+      </c>
+      <c r="E95" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>176</v>
+      </c>
+      <c r="B96" t="s">
+        <v>210</v>
+      </c>
+      <c r="C96" t="s">
+        <v>176</v>
+      </c>
+      <c r="D96" t="s">
+        <v>209</v>
+      </c>
+      <c r="E96" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>177</v>
+      </c>
+      <c r="B97" t="s">
+        <v>210</v>
+      </c>
+      <c r="C97" t="s">
+        <v>177</v>
+      </c>
+      <c r="D97" t="s">
+        <v>209</v>
+      </c>
+      <c r="E97" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" t="s">
+        <v>210</v>
+      </c>
+      <c r="C98" t="s">
+        <v>178</v>
+      </c>
+      <c r="D98" t="s">
+        <v>209</v>
+      </c>
+      <c r="E98" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" t="s">
+        <v>179</v>
+      </c>
+      <c r="D99" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" t="s">
+        <v>210</v>
+      </c>
+      <c r="C100" t="s">
+        <v>180</v>
+      </c>
+      <c r="D100" t="s">
+        <v>209</v>
+      </c>
+      <c r="E100" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>181</v>
+      </c>
+      <c r="B101" t="s">
+        <v>210</v>
+      </c>
+      <c r="C101" t="s">
+        <v>181</v>
+      </c>
+      <c r="D101" t="s">
+        <v>209</v>
+      </c>
+      <c r="E101" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" t="s">
+        <v>210</v>
+      </c>
+      <c r="C102" t="s">
+        <v>182</v>
+      </c>
+      <c r="D102" t="s">
+        <v>209</v>
+      </c>
+      <c r="E102" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>183</v>
+      </c>
+      <c r="B103" t="s">
+        <v>210</v>
+      </c>
+      <c r="C103" t="s">
+        <v>183</v>
+      </c>
+      <c r="D103" t="s">
+        <v>209</v>
+      </c>
+      <c r="E103" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>184</v>
+      </c>
+      <c r="B104" t="s">
+        <v>210</v>
+      </c>
+      <c r="C104" t="s">
+        <v>184</v>
+      </c>
+      <c r="D104" t="s">
+        <v>209</v>
+      </c>
+      <c r="E104" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105" t="s">
+        <v>185</v>
+      </c>
+      <c r="D105" t="s">
+        <v>209</v>
+      </c>
+      <c r="E105" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>186</v>
+      </c>
+      <c r="B106" t="s">
+        <v>210</v>
+      </c>
+      <c r="C106" t="s">
+        <v>186</v>
+      </c>
+      <c r="D106" t="s">
+        <v>209</v>
+      </c>
+      <c r="E106" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>187</v>
+      </c>
+      <c r="B107" t="s">
+        <v>210</v>
+      </c>
+      <c r="C107" t="s">
+        <v>187</v>
+      </c>
+      <c r="D107" t="s">
+        <v>209</v>
+      </c>
+      <c r="E107" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" t="s">
+        <v>188</v>
+      </c>
+      <c r="D108" t="s">
+        <v>209</v>
+      </c>
+      <c r="E108" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>189</v>
+      </c>
+      <c r="B109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C109" t="s">
+        <v>189</v>
+      </c>
+      <c r="D109" t="s">
+        <v>209</v>
+      </c>
+      <c r="E109" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" t="s">
+        <v>210</v>
+      </c>
+      <c r="C110" t="s">
+        <v>190</v>
+      </c>
+      <c r="D110" t="s">
+        <v>209</v>
+      </c>
+      <c r="E110" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>191</v>
+      </c>
+      <c r="B111" t="s">
+        <v>210</v>
+      </c>
+      <c r="C111" t="s">
+        <v>191</v>
+      </c>
+      <c r="D111" t="s">
+        <v>209</v>
+      </c>
+      <c r="E111" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>192</v>
+      </c>
+      <c r="B112" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" t="s">
+        <v>192</v>
+      </c>
+      <c r="D112" t="s">
+        <v>209</v>
+      </c>
+      <c r="E112" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>193</v>
+      </c>
+      <c r="B113" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" t="s">
+        <v>193</v>
+      </c>
+      <c r="D113" t="s">
+        <v>209</v>
+      </c>
+      <c r="E113" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114" t="s">
+        <v>210</v>
+      </c>
+      <c r="C114" t="s">
+        <v>194</v>
+      </c>
+      <c r="D114" t="s">
+        <v>209</v>
+      </c>
+      <c r="E114" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>195</v>
+      </c>
+      <c r="B115" t="s">
+        <v>210</v>
+      </c>
+      <c r="C115" t="s">
+        <v>195</v>
+      </c>
+      <c r="D115" t="s">
+        <v>209</v>
+      </c>
+      <c r="E115" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>196</v>
+      </c>
+      <c r="B116" t="s">
+        <v>210</v>
+      </c>
+      <c r="C116" t="s">
+        <v>196</v>
+      </c>
+      <c r="D116" t="s">
+        <v>209</v>
+      </c>
+      <c r="E116" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>197</v>
+      </c>
+      <c r="B117" t="s">
+        <v>210</v>
+      </c>
+      <c r="C117" t="s">
+        <v>197</v>
+      </c>
+      <c r="D117" t="s">
+        <v>209</v>
+      </c>
+      <c r="E117" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>198</v>
+      </c>
+      <c r="B118" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" t="s">
+        <v>209</v>
+      </c>
+      <c r="E118" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="B119" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="D119" t="s">
+        <v>209</v>
+      </c>
+      <c r="E119" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>199</v>
+      </c>
+      <c r="B120" t="s">
+        <v>210</v>
+      </c>
+      <c r="C120" t="s">
+        <v>199</v>
+      </c>
+      <c r="D120" t="s">
+        <v>209</v>
+      </c>
+      <c r="E120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>200</v>
+      </c>
+      <c r="B121" t="s">
+        <v>210</v>
+      </c>
+      <c r="C121" t="s">
+        <v>200</v>
+      </c>
+      <c r="D121" t="s">
+        <v>209</v>
+      </c>
+      <c r="E121" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>201</v>
+      </c>
+      <c r="B122" t="s">
+        <v>210</v>
+      </c>
+      <c r="C122" t="s">
+        <v>201</v>
+      </c>
+      <c r="D122" t="s">
+        <v>209</v>
+      </c>
+      <c r="E122" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>202</v>
+      </c>
+      <c r="B123" t="s">
+        <v>210</v>
+      </c>
+      <c r="C123" t="s">
+        <v>202</v>
+      </c>
+      <c r="D123" t="s">
+        <v>209</v>
+      </c>
+      <c r="E123" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" t="s">
+        <v>203</v>
+      </c>
+      <c r="D124" t="s">
+        <v>209</v>
+      </c>
+      <c r="E124" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>204</v>
+      </c>
+      <c r="B125" t="s">
+        <v>210</v>
+      </c>
+      <c r="C125" t="s">
+        <v>204</v>
+      </c>
+      <c r="D125" t="s">
+        <v>209</v>
+      </c>
+      <c r="E125" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>205</v>
+      </c>
+      <c r="B126" t="s">
+        <v>210</v>
+      </c>
+      <c r="C126" t="s">
+        <v>205</v>
+      </c>
+      <c r="D126" t="s">
+        <v>209</v>
+      </c>
+      <c r="E126" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>206</v>
+      </c>
+      <c r="B127" t="s">
+        <v>210</v>
+      </c>
+      <c r="C127" t="s">
+        <v>206</v>
+      </c>
+      <c r="D127" t="s">
+        <v>209</v>
+      </c>
+      <c r="E127" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>207</v>
+      </c>
+      <c r="B128" t="s">
+        <v>210</v>
+      </c>
+      <c r="C128" t="s">
+        <v>207</v>
+      </c>
+      <c r="D128" t="s">
+        <v>209</v>
+      </c>
+      <c r="E128" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>208</v>
+      </c>
+      <c r="B129" t="s">
+        <v>210</v>
+      </c>
+      <c r="C129" t="s">
+        <v>208</v>
+      </c>
+      <c r="D129" t="s">
+        <v>209</v>
+      </c>
+      <c r="E129" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:06:30
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAEFDA-893A-4645-9F8C-D1DC74889EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710EF544-648D-4FA7-BF4C-A614D14BF2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="253">
   <si>
     <t>Host</t>
   </si>
@@ -624,36 +624,6 @@
     <t>172.16.91.7</t>
   </si>
   <si>
-    <t>172.16.11.7</t>
-  </si>
-  <si>
-    <t>172.16.3.6</t>
-  </si>
-  <si>
-    <t>172.16.107.7</t>
-  </si>
-  <si>
-    <t>172.16.116.80</t>
-  </si>
-  <si>
-    <t>10.16.77.4</t>
-  </si>
-  <si>
-    <t>10.173.3.7</t>
-  </si>
-  <si>
-    <t>10.121.0.6</t>
-  </si>
-  <si>
-    <t>172.16.134.4</t>
-  </si>
-  <si>
-    <t>10.125.3.8</t>
-  </si>
-  <si>
-    <t>10.245.3.4</t>
-  </si>
-  <si>
     <t>ansible_test</t>
   </si>
   <si>
@@ -790,39 +760,6 @@
   </si>
   <si>
     <t>akigp-bk</t>
-  </si>
-  <si>
-    <t>akb30-n1</t>
-  </si>
-  <si>
-    <t>akb68-n1</t>
-  </si>
-  <si>
-    <t>akvil-n1</t>
-  </si>
-  <si>
-    <t>akbar-bk</t>
-  </si>
-  <si>
-    <t>aksin-bk</t>
-  </si>
-  <si>
-    <t>akcan-n1</t>
-  </si>
-  <si>
-    <t>alapa-bk</t>
-  </si>
-  <si>
-    <t>akyop-n1</t>
-  </si>
-  <si>
-    <t>akede-n1</t>
-  </si>
-  <si>
-    <t>albu2-bk</t>
-  </si>
-  <si>
-    <t>ktnqs-n1</t>
   </si>
   <si>
     <t>alba5-bk</t>
@@ -902,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,9 +852,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2429,70 +2363,70 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B71" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C71" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="D71" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E71" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B72" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C72" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="D72" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E72" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C73" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="D73" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E73" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C74" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="D74" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E74" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,16 +2434,16 @@
         <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C75" t="s">
         <v>155</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E75" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,16 +2451,16 @@
         <v>156</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C76" t="s">
         <v>156</v>
       </c>
       <c r="D76" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E76" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,16 +2468,16 @@
         <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C77" t="s">
         <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E77" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2551,16 +2485,16 @@
         <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C78" t="s">
         <v>158</v>
       </c>
       <c r="D78" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E78" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,16 +2502,16 @@
         <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C79" t="s">
         <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E79" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2585,16 +2519,16 @@
         <v>160</v>
       </c>
       <c r="B80" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C80" t="s">
         <v>160</v>
       </c>
       <c r="D80" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E80" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2602,16 +2536,16 @@
         <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C81" t="s">
         <v>161</v>
       </c>
       <c r="D81" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E81" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2619,16 +2553,16 @@
         <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C82" t="s">
         <v>162</v>
       </c>
       <c r="D82" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E82" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,16 +2570,16 @@
         <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C83" t="s">
         <v>163</v>
       </c>
       <c r="D83" t="s">
+        <v>199</v>
+      </c>
+      <c r="E83" t="s">
         <v>209</v>
-      </c>
-      <c r="E83" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2653,16 +2587,16 @@
         <v>164</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C84" t="s">
         <v>164</v>
       </c>
       <c r="D84" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E84" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2670,16 +2604,16 @@
         <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C85" t="s">
         <v>165</v>
       </c>
       <c r="D85" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E85" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2687,16 +2621,16 @@
         <v>166</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C86" t="s">
         <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E86" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,16 +2638,16 @@
         <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C87" t="s">
         <v>167</v>
       </c>
       <c r="D87" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E87" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2721,16 +2655,16 @@
         <v>168</v>
       </c>
       <c r="B88" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C88" t="s">
         <v>168</v>
       </c>
       <c r="D88" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E88" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2738,16 +2672,16 @@
         <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C89" t="s">
         <v>169</v>
       </c>
       <c r="D89" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E89" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2755,16 +2689,16 @@
         <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C90" t="s">
         <v>170</v>
       </c>
       <c r="D90" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E90" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2772,16 +2706,16 @@
         <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C91" t="s">
         <v>171</v>
       </c>
       <c r="D91" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E91" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,16 +2723,16 @@
         <v>172</v>
       </c>
       <c r="B92" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C92" t="s">
         <v>172</v>
       </c>
       <c r="D92" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E92" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2806,16 +2740,16 @@
         <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
         <v>173</v>
       </c>
       <c r="D93" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E93" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2823,16 +2757,16 @@
         <v>174</v>
       </c>
       <c r="B94" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C94" t="s">
         <v>174</v>
       </c>
       <c r="D94" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E94" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2840,16 +2774,16 @@
         <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C95" t="s">
         <v>175</v>
       </c>
       <c r="D95" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E95" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2857,16 +2791,16 @@
         <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C96" t="s">
         <v>176</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E96" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2874,16 +2808,16 @@
         <v>177</v>
       </c>
       <c r="B97" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C97" t="s">
         <v>177</v>
       </c>
       <c r="D97" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E97" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2891,16 +2825,16 @@
         <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C98" t="s">
         <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E98" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2908,16 +2842,16 @@
         <v>179</v>
       </c>
       <c r="B99" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C99" t="s">
         <v>179</v>
       </c>
       <c r="D99" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E99" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2925,16 +2859,16 @@
         <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C100" t="s">
         <v>180</v>
       </c>
       <c r="D100" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E100" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,16 +2876,16 @@
         <v>181</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C101" t="s">
         <v>181</v>
       </c>
       <c r="D101" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E101" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2959,16 +2893,16 @@
         <v>182</v>
       </c>
       <c r="B102" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C102" t="s">
         <v>182</v>
       </c>
       <c r="D102" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E102" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2976,16 +2910,16 @@
         <v>183</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C103" t="s">
         <v>183</v>
       </c>
       <c r="D103" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E103" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2993,16 +2927,16 @@
         <v>184</v>
       </c>
       <c r="B104" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C104" t="s">
         <v>184</v>
       </c>
       <c r="D104" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E104" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3010,16 +2944,16 @@
         <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C105" t="s">
         <v>185</v>
       </c>
       <c r="D105" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E105" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3027,16 +2961,16 @@
         <v>186</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C106" t="s">
         <v>186</v>
       </c>
       <c r="D106" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E106" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,16 +2978,16 @@
         <v>187</v>
       </c>
       <c r="B107" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C107" t="s">
         <v>187</v>
       </c>
       <c r="D107" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E107" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,16 +2995,16 @@
         <v>188</v>
       </c>
       <c r="B108" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C108" t="s">
         <v>188</v>
       </c>
       <c r="D108" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E108" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3078,16 +3012,16 @@
         <v>189</v>
       </c>
       <c r="B109" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C109" t="s">
         <v>189</v>
       </c>
       <c r="D109" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E109" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,16 +3029,16 @@
         <v>190</v>
       </c>
       <c r="B110" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C110" t="s">
         <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E110" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,16 +3046,16 @@
         <v>191</v>
       </c>
       <c r="B111" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C111" t="s">
         <v>191</v>
       </c>
       <c r="D111" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E111" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3129,16 +3063,16 @@
         <v>192</v>
       </c>
       <c r="B112" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C112" t="s">
         <v>192</v>
       </c>
       <c r="D112" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E112" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3146,16 +3080,16 @@
         <v>193</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C113" t="s">
         <v>193</v>
       </c>
       <c r="D113" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E113" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3163,16 +3097,16 @@
         <v>194</v>
       </c>
       <c r="B114" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C114" t="s">
         <v>194</v>
       </c>
       <c r="D114" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E114" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3180,16 +3114,16 @@
         <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C115" t="s">
         <v>195</v>
       </c>
       <c r="D115" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E115" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3197,16 +3131,16 @@
         <v>196</v>
       </c>
       <c r="B116" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C116" t="s">
         <v>196</v>
       </c>
       <c r="D116" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E116" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3214,16 +3148,16 @@
         <v>197</v>
       </c>
       <c r="B117" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C117" t="s">
         <v>197</v>
       </c>
       <c r="D117" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E117" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3231,203 +3165,16 @@
         <v>198</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C118" t="s">
         <v>198</v>
       </c>
       <c r="D118" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E118" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="6">
-        <v>147127110112</v>
-      </c>
-      <c r="B119" t="s">
-        <v>210</v>
-      </c>
-      <c r="C119" s="6">
-        <v>147127110112</v>
-      </c>
-      <c r="D119" t="s">
-        <v>209</v>
-      </c>
-      <c r="E119" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>199</v>
-      </c>
-      <c r="B120" t="s">
-        <v>210</v>
-      </c>
-      <c r="C120" t="s">
-        <v>199</v>
-      </c>
-      <c r="D120" t="s">
-        <v>209</v>
-      </c>
-      <c r="E120" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>200</v>
-      </c>
-      <c r="B121" t="s">
-        <v>210</v>
-      </c>
-      <c r="C121" t="s">
-        <v>200</v>
-      </c>
-      <c r="D121" t="s">
-        <v>209</v>
-      </c>
-      <c r="E121" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>201</v>
-      </c>
-      <c r="B122" t="s">
-        <v>210</v>
-      </c>
-      <c r="C122" t="s">
-        <v>201</v>
-      </c>
-      <c r="D122" t="s">
-        <v>209</v>
-      </c>
-      <c r="E122" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>202</v>
-      </c>
-      <c r="B123" t="s">
-        <v>210</v>
-      </c>
-      <c r="C123" t="s">
-        <v>202</v>
-      </c>
-      <c r="D123" t="s">
-        <v>209</v>
-      </c>
-      <c r="E123" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>203</v>
-      </c>
-      <c r="B124" t="s">
-        <v>210</v>
-      </c>
-      <c r="C124" t="s">
-        <v>203</v>
-      </c>
-      <c r="D124" t="s">
-        <v>209</v>
-      </c>
-      <c r="E124" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>204</v>
-      </c>
-      <c r="B125" t="s">
-        <v>210</v>
-      </c>
-      <c r="C125" t="s">
-        <v>204</v>
-      </c>
-      <c r="D125" t="s">
-        <v>209</v>
-      </c>
-      <c r="E125" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>205</v>
-      </c>
-      <c r="B126" t="s">
-        <v>210</v>
-      </c>
-      <c r="C126" t="s">
-        <v>205</v>
-      </c>
-      <c r="D126" t="s">
-        <v>209</v>
-      </c>
-      <c r="E126" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>206</v>
-      </c>
-      <c r="B127" t="s">
-        <v>210</v>
-      </c>
-      <c r="C127" t="s">
-        <v>206</v>
-      </c>
-      <c r="D127" t="s">
-        <v>209</v>
-      </c>
-      <c r="E127" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>207</v>
-      </c>
-      <c r="B128" t="s">
-        <v>210</v>
-      </c>
-      <c r="C128" t="s">
-        <v>207</v>
-      </c>
-      <c r="D128" t="s">
-        <v>209</v>
-      </c>
-      <c r="E128" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>208</v>
-      </c>
-      <c r="B129" t="s">
-        <v>210</v>
-      </c>
-      <c r="C129" t="s">
-        <v>208</v>
-      </c>
-      <c r="D129" t="s">
-        <v>209</v>
-      </c>
-      <c r="E129" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:07:31
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710EF544-648D-4FA7-BF4C-A614D14BF2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340D9EC-C6E4-4F4D-8B05-A364B9F8FCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="273">
   <si>
     <t>Host</t>
   </si>
@@ -624,6 +624,36 @@
     <t>172.16.91.7</t>
   </si>
   <si>
+    <t>172.16.11.7</t>
+  </si>
+  <si>
+    <t>172.16.3.6</t>
+  </si>
+  <si>
+    <t>172.16.107.7</t>
+  </si>
+  <si>
+    <t>172.16.116.80</t>
+  </si>
+  <si>
+    <t>10.16.77.4</t>
+  </si>
+  <si>
+    <t>10.173.3.7</t>
+  </si>
+  <si>
+    <t>10.121.0.6</t>
+  </si>
+  <si>
+    <t>172.16.134.4</t>
+  </si>
+  <si>
+    <t>10.125.3.8</t>
+  </si>
+  <si>
+    <t>10.245.3.4</t>
+  </si>
+  <si>
     <t>ansible_test</t>
   </si>
   <si>
@@ -760,6 +790,36 @@
   </si>
   <si>
     <t>akigp-bk</t>
+  </si>
+  <si>
+    <t>akb68-n1</t>
+  </si>
+  <si>
+    <t>akvil-n1</t>
+  </si>
+  <si>
+    <t>akbar-bk</t>
+  </si>
+  <si>
+    <t>aksin-bk</t>
+  </si>
+  <si>
+    <t>akcan-n1</t>
+  </si>
+  <si>
+    <t>alapa-bk</t>
+  </si>
+  <si>
+    <t>akyop-n1</t>
+  </si>
+  <si>
+    <t>akede-n1</t>
+  </si>
+  <si>
+    <t>albu2-bk</t>
+  </si>
+  <si>
+    <t>ktnqs-n1</t>
   </si>
   <si>
     <t>alba5-bk</t>
@@ -1132,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,70 +2423,70 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C71" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="D71" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E71" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B72" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D72" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E72" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="B73" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D73" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E73" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B74" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D74" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E74" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,16 +2494,16 @@
         <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C75" t="s">
         <v>155</v>
       </c>
       <c r="D75" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2451,16 +2511,16 @@
         <v>156</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C76" t="s">
         <v>156</v>
       </c>
       <c r="D76" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E76" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2468,16 +2528,16 @@
         <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
         <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E77" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2485,16 +2545,16 @@
         <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C78" t="s">
         <v>158</v>
       </c>
       <c r="D78" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E78" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2502,16 +2562,16 @@
         <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C79" t="s">
         <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E79" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2519,16 +2579,16 @@
         <v>160</v>
       </c>
       <c r="B80" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C80" t="s">
         <v>160</v>
       </c>
       <c r="D80" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E80" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,16 +2596,16 @@
         <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C81" t="s">
         <v>161</v>
       </c>
       <c r="D81" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E81" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2553,16 +2613,16 @@
         <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C82" t="s">
         <v>162</v>
       </c>
       <c r="D82" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E82" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,16 +2630,16 @@
         <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C83" t="s">
         <v>163</v>
       </c>
       <c r="D83" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E83" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2587,16 +2647,16 @@
         <v>164</v>
       </c>
       <c r="B84" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C84" t="s">
         <v>164</v>
       </c>
       <c r="D84" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E84" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,16 +2664,16 @@
         <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C85" t="s">
         <v>165</v>
       </c>
       <c r="D85" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E85" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,16 +2681,16 @@
         <v>166</v>
       </c>
       <c r="B86" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C86" t="s">
         <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,16 +2698,16 @@
         <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C87" t="s">
         <v>167</v>
       </c>
       <c r="D87" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2655,16 +2715,16 @@
         <v>168</v>
       </c>
       <c r="B88" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C88" t="s">
         <v>168</v>
       </c>
       <c r="D88" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2672,16 +2732,16 @@
         <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C89" t="s">
         <v>169</v>
       </c>
       <c r="D89" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E89" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,16 +2749,16 @@
         <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C90" t="s">
         <v>170</v>
       </c>
       <c r="D90" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E90" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2706,16 +2766,16 @@
         <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C91" t="s">
         <v>171</v>
       </c>
       <c r="D91" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E91" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2723,16 +2783,16 @@
         <v>172</v>
       </c>
       <c r="B92" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C92" t="s">
         <v>172</v>
       </c>
       <c r="D92" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E92" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2740,16 +2800,16 @@
         <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C93" t="s">
         <v>173</v>
       </c>
       <c r="D93" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E93" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2757,16 +2817,16 @@
         <v>174</v>
       </c>
       <c r="B94" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C94" t="s">
         <v>174</v>
       </c>
       <c r="D94" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E94" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,16 +2834,16 @@
         <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C95" t="s">
         <v>175</v>
       </c>
       <c r="D95" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E95" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,16 +2851,16 @@
         <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C96" t="s">
         <v>176</v>
       </c>
       <c r="D96" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E96" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,16 +2868,16 @@
         <v>177</v>
       </c>
       <c r="B97" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C97" t="s">
         <v>177</v>
       </c>
       <c r="D97" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E97" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,16 +2885,16 @@
         <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C98" t="s">
         <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E98" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2842,16 +2902,16 @@
         <v>179</v>
       </c>
       <c r="B99" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C99" t="s">
         <v>179</v>
       </c>
       <c r="D99" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E99" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2859,16 +2919,16 @@
         <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C100" t="s">
         <v>180</v>
       </c>
       <c r="D100" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E100" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,16 +2936,16 @@
         <v>181</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C101" t="s">
         <v>181</v>
       </c>
       <c r="D101" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E101" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2893,16 +2953,16 @@
         <v>182</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C102" t="s">
         <v>182</v>
       </c>
       <c r="D102" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E102" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,16 +2970,16 @@
         <v>183</v>
       </c>
       <c r="B103" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C103" t="s">
         <v>183</v>
       </c>
       <c r="D103" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E103" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2927,16 +2987,16 @@
         <v>184</v>
       </c>
       <c r="B104" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C104" t="s">
         <v>184</v>
       </c>
       <c r="D104" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E104" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2944,16 +3004,16 @@
         <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C105" t="s">
         <v>185</v>
       </c>
       <c r="D105" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E105" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2961,16 +3021,16 @@
         <v>186</v>
       </c>
       <c r="B106" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C106" t="s">
         <v>186</v>
       </c>
       <c r="D106" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E106" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2978,16 +3038,16 @@
         <v>187</v>
       </c>
       <c r="B107" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C107" t="s">
         <v>187</v>
       </c>
       <c r="D107" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E107" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2995,16 +3055,16 @@
         <v>188</v>
       </c>
       <c r="B108" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C108" t="s">
         <v>188</v>
       </c>
       <c r="D108" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E108" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3072,16 @@
         <v>189</v>
       </c>
       <c r="B109" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C109" t="s">
         <v>189</v>
       </c>
       <c r="D109" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,16 +3089,16 @@
         <v>190</v>
       </c>
       <c r="B110" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C110" t="s">
         <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E110" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3106,16 @@
         <v>191</v>
       </c>
       <c r="B111" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C111" t="s">
         <v>191</v>
       </c>
       <c r="D111" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E111" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3063,16 +3123,16 @@
         <v>192</v>
       </c>
       <c r="B112" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C112" t="s">
         <v>192</v>
       </c>
       <c r="D112" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E112" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3080,16 +3140,16 @@
         <v>193</v>
       </c>
       <c r="B113" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C113" t="s">
         <v>193</v>
       </c>
       <c r="D113" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E113" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3157,16 @@
         <v>194</v>
       </c>
       <c r="B114" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C114" t="s">
         <v>194</v>
       </c>
       <c r="D114" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E114" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3174,16 @@
         <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C115" t="s">
         <v>195</v>
       </c>
       <c r="D115" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E115" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3191,16 @@
         <v>196</v>
       </c>
       <c r="B116" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C116" t="s">
         <v>196</v>
       </c>
       <c r="D116" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E116" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,16 +3208,16 @@
         <v>197</v>
       </c>
       <c r="B117" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C117" t="s">
         <v>197</v>
       </c>
       <c r="D117" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E117" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,16 +3225,186 @@
         <v>198</v>
       </c>
       <c r="B118" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C118" t="s">
         <v>198</v>
       </c>
       <c r="D118" t="s">
+        <v>209</v>
+      </c>
+      <c r="E118" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>199</v>
       </c>
-      <c r="E118" t="s">
-        <v>244</v>
+      <c r="B119" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" t="s">
+        <v>199</v>
+      </c>
+      <c r="D119" t="s">
+        <v>209</v>
+      </c>
+      <c r="E119" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>200</v>
+      </c>
+      <c r="B120" t="s">
+        <v>210</v>
+      </c>
+      <c r="C120" t="s">
+        <v>200</v>
+      </c>
+      <c r="D120" t="s">
+        <v>209</v>
+      </c>
+      <c r="E120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>201</v>
+      </c>
+      <c r="B121" t="s">
+        <v>210</v>
+      </c>
+      <c r="C121" t="s">
+        <v>201</v>
+      </c>
+      <c r="D121" t="s">
+        <v>209</v>
+      </c>
+      <c r="E121" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>202</v>
+      </c>
+      <c r="B122" t="s">
+        <v>210</v>
+      </c>
+      <c r="C122" t="s">
+        <v>202</v>
+      </c>
+      <c r="D122" t="s">
+        <v>209</v>
+      </c>
+      <c r="E122" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>203</v>
+      </c>
+      <c r="B123" t="s">
+        <v>210</v>
+      </c>
+      <c r="C123" t="s">
+        <v>203</v>
+      </c>
+      <c r="D123" t="s">
+        <v>209</v>
+      </c>
+      <c r="E123" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>204</v>
+      </c>
+      <c r="B124" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" t="s">
+        <v>204</v>
+      </c>
+      <c r="D124" t="s">
+        <v>209</v>
+      </c>
+      <c r="E124" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>205</v>
+      </c>
+      <c r="B125" t="s">
+        <v>210</v>
+      </c>
+      <c r="C125" t="s">
+        <v>205</v>
+      </c>
+      <c r="D125" t="s">
+        <v>209</v>
+      </c>
+      <c r="E125" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>206</v>
+      </c>
+      <c r="B126" t="s">
+        <v>210</v>
+      </c>
+      <c r="C126" t="s">
+        <v>206</v>
+      </c>
+      <c r="D126" t="s">
+        <v>209</v>
+      </c>
+      <c r="E126" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>207</v>
+      </c>
+      <c r="B127" t="s">
+        <v>210</v>
+      </c>
+      <c r="C127" t="s">
+        <v>207</v>
+      </c>
+      <c r="D127" t="s">
+        <v>209</v>
+      </c>
+      <c r="E127" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>208</v>
+      </c>
+      <c r="B128" t="s">
+        <v>210</v>
+      </c>
+      <c r="C128" t="s">
+        <v>208</v>
+      </c>
+      <c r="D128" t="s">
+        <v>209</v>
+      </c>
+      <c r="E128" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:11:43
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340D9EC-C6E4-4F4D-8B05-A364B9F8FCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BBD496-E42A-4C29-A692-60DF5A11878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
   <si>
     <t>Host</t>
   </si>
@@ -790,6 +790,9 @@
   </si>
   <si>
     <t>akigp-bk</t>
+  </si>
+  <si>
+    <t>akb30-n1</t>
   </si>
   <si>
     <t>akb68-n1</t>
@@ -899,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -912,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,70 +2429,70 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B71" t="s">
         <v>210</v>
       </c>
       <c r="C71" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D71" t="s">
         <v>209</v>
       </c>
       <c r="E71" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B72" t="s">
         <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D72" t="s">
         <v>209</v>
       </c>
       <c r="E72" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B73" t="s">
         <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D73" t="s">
         <v>209</v>
       </c>
       <c r="E73" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B74" t="s">
         <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D74" t="s">
         <v>209</v>
       </c>
       <c r="E74" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3251,7 +3257,7 @@
         <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3268,7 +3274,7 @@
         <v>209</v>
       </c>
       <c r="E120" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3285,7 +3291,7 @@
         <v>209</v>
       </c>
       <c r="E121" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3302,7 +3308,7 @@
         <v>209</v>
       </c>
       <c r="E122" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3319,7 +3325,7 @@
         <v>209</v>
       </c>
       <c r="E123" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3336,7 +3342,7 @@
         <v>209</v>
       </c>
       <c r="E124" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3353,7 +3359,7 @@
         <v>209</v>
       </c>
       <c r="E125" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3376,7 @@
         <v>209</v>
       </c>
       <c r="E126" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,7 +3393,7 @@
         <v>209</v>
       </c>
       <c r="E127" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3404,7 +3410,24 @@
         <v>209</v>
       </c>
       <c r="E128" t="s">
-        <v>264</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="B129" t="s">
+        <v>210</v>
+      </c>
+      <c r="C129" s="6">
+        <v>147127110112</v>
+      </c>
+      <c r="D129" t="s">
+        <v>209</v>
+      </c>
+      <c r="E129" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:13:11
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BBD496-E42A-4C29-A692-60DF5A11878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF6E496-F81F-4CB8-BD91-B97D6909378A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -915,9 +915,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,7 +1199,7 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:15:42
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF6E496-F81F-4CB8-BD91-B97D6909378A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C7ECA3-CC5B-49BB-991B-B893E1678C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,7 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1199,7 +1198,7 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3412,13 +3411,13 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="6">
+      <c r="A129">
         <v>147127110112</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129" s="6">
+      <c r="C129">
         <v>147127110112</v>
       </c>
       <c r="D129" t="s">

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:17:03
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C7ECA3-CC5B-49BB-991B-B893E1678C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C8A525-4FB6-4B6B-8D52-59656E3571E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,12 +1201,12 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" customWidth="1"/>
@@ -3411,13 +3414,13 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129">
+      <c r="A129" s="6">
         <v>147127110112</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="6">
         <v>147127110112</v>
       </c>
       <c r="D129" t="s">

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:20:10
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C8A525-4FB6-4B6B-8D52-59656E3571E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB92EF9-B59D-4624-B10F-63D35FBAE268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,9 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3414,13 +3411,13 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="6">
+      <c r="A129">
         <v>147127110112</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129" s="6">
+      <c r="C129">
         <v>147127110112</v>
       </c>
       <c r="D129" t="s">

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:24:02
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB92EF9-B59D-4624-B10F-63D35FBAE268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF20C03-59FD-4359-B40B-8376D062A81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,7 +1201,7 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,13 +3414,13 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129">
+      <c r="A129" s="6">
         <v>147127110112</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="6">
         <v>147127110112</v>
       </c>
       <c r="D129" t="s">

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:26:57
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF20C03-59FD-4359-B40B-8376D062A81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3418E1-5442-421B-A91F-40F8B2D7639E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="275">
   <si>
     <t>Host</t>
   </si>
@@ -847,6 +847,9 @@
   </si>
   <si>
     <t>10.106.3.4</t>
+  </si>
+  <si>
+    <t>147.127.110.112</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1204,7 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3414,14 +3417,14 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="6">
-        <v>147127110112</v>
+      <c r="A129" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129" s="6">
-        <v>147127110112</v>
+      <c r="C129" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="D129" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 17:30:15
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3418E1-5442-421B-A91F-40F8B2D7639E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA84EA1-1588-4415-9F8A-7D3EA79D2AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="276">
   <si>
     <t>Host</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>147.127.110.112</t>
+  </si>
+  <si>
+    <t>Srv_Geo_Bk -Problem</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,7 +3203,7 @@
         <v>196</v>
       </c>
       <c r="B116" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="C116" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 18:28:29
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\7\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\13\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA84EA1-1588-4415-9F8A-7D3EA79D2AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5BE12B-7D75-479D-BA84-0B12E2281906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="277">
   <si>
     <t>Host</t>
   </si>
@@ -852,7 +852,10 @@
     <t>147.127.110.112</t>
   </si>
   <si>
-    <t>Srv_Geo_Bk -Problem</t>
+    <t xml:space="preserve">Srv_Geo_Bk </t>
+  </si>
+  <si>
+    <t>Srv_Geo_Bk - problem</t>
   </si>
 </sst>
 </file>
@@ -921,7 +924,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1206,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,7 +2917,7 @@
         <v>179</v>
       </c>
       <c r="B99" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="C99" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-17 18:30:35
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\13\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5BE12B-7D75-479D-BA84-0B12E2281906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF68748A-22A6-49D3-BBBC-24F95FABD55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="278">
   <si>
     <t>Host</t>
   </si>
@@ -856,6 +856,9 @@
   </si>
   <si>
     <t>Srv_Geo_Bk - problem</t>
+  </si>
+  <si>
+    <t>172.16.77.4</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3331,7 @@
         <v>210</v>
       </c>
       <c r="C123" t="s">
-        <v>203</v>
+        <v>277</v>
       </c>
       <c r="D123" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-21 10:50:08
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\13\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79958935\AppData\Local\Temp\scp43155\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF68748A-22A6-49D3-BBBC-24F95FABD55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CA8245-E969-473A-8285-4BB237B9B93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="282">
   <si>
     <t>Host</t>
   </si>
@@ -859,6 +859,18 @@
   </si>
   <si>
     <t>172.16.77.4</t>
+  </si>
+  <si>
+    <t>10.181.5.214</t>
+  </si>
+  <si>
+    <t>contactcrmdbprd</t>
+  </si>
+  <si>
+    <t>10.181.5.219</t>
+  </si>
+  <si>
+    <t>crmdb4</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3442,6 +3454,40 @@
         <v>255</v>
       </c>
     </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>278</v>
+      </c>
+      <c r="B130" t="s">
+        <v>148</v>
+      </c>
+      <c r="C130" t="s">
+        <v>278</v>
+      </c>
+      <c r="D130" t="s">
+        <v>209</v>
+      </c>
+      <c r="E130" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>280</v>
+      </c>
+      <c r="B131" t="s">
+        <v>148</v>
+      </c>
+      <c r="C131" t="s">
+        <v>280</v>
+      </c>
+      <c r="D131" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-03-21 14:31:21
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79958935\AppData\Local\Temp\scp43155\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79958935\AppData\Local\Temp\scp27045\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CA8245-E969-473A-8285-4BB237B9B93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA6B666-12BD-45CC-8D4C-3134F7491DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,7 +3465,7 @@
         <v>278</v>
       </c>
       <c r="D130" t="s">
-        <v>209</v>
+        <v>97</v>
       </c>
       <c r="E130" t="s">
         <v>279</v>
@@ -3482,7 +3482,7 @@
         <v>280</v>
       </c>
       <c r="D131" t="s">
-        <v>209</v>
+        <v>97</v>
       </c>
       <c r="E131" t="s">
         <v>281</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-04-14 08:50:24
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79958935\AppData\Local\Temp\scp27045\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp44351\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA6B666-12BD-45CC-8D4C-3134F7491DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2976E6A3-0355-4DDF-B4E2-4A588F81910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="284">
   <si>
     <t>Host</t>
   </si>
@@ -871,6 +871,12 @@
   </si>
   <si>
     <t>crmdb4</t>
+  </si>
+  <si>
+    <t>10.181.11.98</t>
+  </si>
+  <si>
+    <t>central-qa3</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,1512 +1985,1535 @@
       <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="B46" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>101</v>
+      <c r="C46" t="s">
+        <v>98</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
         <v>99</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B54" t="s">
         <v>99</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
         <v>99</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
         <v>150</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="B58" t="s">
         <v>150</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>125</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
         <v>150</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
         <v>150</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
         <v>150</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B63" t="s">
         <v>150</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
         <v>150</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
         <v>150</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B66" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
         <v>146</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D69" t="s">
         <v>97</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" t="s">
-        <v>152</v>
+        <v>146</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E72" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>270</v>
-      </c>
-      <c r="B71" t="s">
-        <v>210</v>
-      </c>
-      <c r="C71" t="s">
-        <v>270</v>
-      </c>
-      <c r="D71" t="s">
-        <v>209</v>
-      </c>
-      <c r="E71" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>271</v>
-      </c>
-      <c r="B72" t="s">
-        <v>210</v>
-      </c>
-      <c r="C72" t="s">
-        <v>271</v>
-      </c>
-      <c r="D72" t="s">
-        <v>209</v>
-      </c>
-      <c r="E72" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B73" t="s">
         <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D73" t="s">
         <v>209</v>
       </c>
       <c r="E73" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B74" t="s">
         <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D74" t="s">
         <v>209</v>
       </c>
       <c r="E74" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>272</v>
       </c>
       <c r="B75" t="s">
         <v>210</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>272</v>
       </c>
       <c r="D75" t="s">
         <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>211</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>273</v>
       </c>
       <c r="B76" t="s">
         <v>210</v>
       </c>
       <c r="C76" t="s">
-        <v>156</v>
+        <v>273</v>
       </c>
       <c r="D76" t="s">
         <v>209</v>
       </c>
       <c r="E76" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
         <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D77" t="s">
         <v>209</v>
       </c>
       <c r="E77" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B78" t="s">
         <v>210</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
         <v>209</v>
       </c>
       <c r="E78" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
         <v>210</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D79" t="s">
         <v>209</v>
       </c>
       <c r="E79" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
         <v>210</v>
       </c>
       <c r="C80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D80" t="s">
         <v>209</v>
       </c>
       <c r="E80" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
         <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D81" t="s">
         <v>209</v>
       </c>
       <c r="E81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B82" t="s">
         <v>210</v>
       </c>
       <c r="C82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D82" t="s">
         <v>209</v>
       </c>
       <c r="E82" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
         <v>210</v>
       </c>
       <c r="C83" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D83" t="s">
         <v>209</v>
       </c>
       <c r="E83" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
         <v>210</v>
       </c>
       <c r="C84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D84" t="s">
         <v>209</v>
       </c>
       <c r="E84" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
         <v>210</v>
       </c>
       <c r="C85" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D85" t="s">
         <v>209</v>
       </c>
       <c r="E85" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
         <v>210</v>
       </c>
       <c r="C86" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D86" t="s">
         <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B87" t="s">
         <v>210</v>
       </c>
       <c r="C87" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D87" t="s">
         <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
         <v>210</v>
       </c>
       <c r="C88" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
         <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
         <v>210</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D89" t="s">
         <v>209</v>
       </c>
       <c r="E89" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
         <v>210</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D90" t="s">
         <v>209</v>
       </c>
       <c r="E90" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
         <v>210</v>
       </c>
       <c r="C91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D91" t="s">
         <v>209</v>
       </c>
       <c r="E91" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B92" t="s">
         <v>210</v>
       </c>
       <c r="C92" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D92" t="s">
         <v>209</v>
       </c>
       <c r="E92" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B93" t="s">
         <v>210</v>
       </c>
       <c r="C93" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D93" t="s">
         <v>209</v>
       </c>
       <c r="E93" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B94" t="s">
         <v>210</v>
       </c>
       <c r="C94" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D94" t="s">
         <v>209</v>
       </c>
       <c r="E94" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B95" t="s">
         <v>210</v>
       </c>
       <c r="C95" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D95" t="s">
         <v>209</v>
       </c>
       <c r="E95" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
         <v>210</v>
       </c>
       <c r="C96" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D96" t="s">
         <v>209</v>
       </c>
       <c r="E96" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
         <v>210</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D97" t="s">
         <v>209</v>
       </c>
       <c r="E97" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
         <v>210</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D98" t="s">
         <v>209</v>
       </c>
       <c r="E98" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B99" t="s">
-        <v>276</v>
+        <v>210</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D99" t="s">
         <v>209</v>
       </c>
       <c r="E99" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B100" t="s">
         <v>210</v>
       </c>
       <c r="C100" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D100" t="s">
         <v>209</v>
       </c>
       <c r="E100" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="C101" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D101" t="s">
         <v>209</v>
       </c>
       <c r="E101" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B102" t="s">
         <v>210</v>
       </c>
       <c r="C102" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D102" t="s">
         <v>209</v>
       </c>
       <c r="E102" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
         <v>210</v>
       </c>
       <c r="C103" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D103" t="s">
         <v>209</v>
       </c>
       <c r="E103" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
         <v>210</v>
       </c>
       <c r="C104" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D104" t="s">
         <v>209</v>
       </c>
       <c r="E104" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
         <v>210</v>
       </c>
       <c r="C105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D105" t="s">
         <v>209</v>
       </c>
       <c r="E105" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
         <v>210</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D106" t="s">
         <v>209</v>
       </c>
       <c r="E106" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
         <v>210</v>
       </c>
       <c r="C107" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D107" t="s">
         <v>209</v>
       </c>
       <c r="E107" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B108" t="s">
         <v>210</v>
       </c>
       <c r="C108" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D108" t="s">
         <v>209</v>
       </c>
       <c r="E108" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B109" t="s">
         <v>210</v>
       </c>
       <c r="C109" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D109" t="s">
         <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B110" t="s">
         <v>210</v>
       </c>
       <c r="C110" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D110" t="s">
         <v>209</v>
       </c>
       <c r="E110" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B111" t="s">
         <v>210</v>
       </c>
       <c r="C111" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D111" t="s">
         <v>209</v>
       </c>
       <c r="E111" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B112" t="s">
         <v>210</v>
       </c>
       <c r="C112" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D112" t="s">
         <v>209</v>
       </c>
       <c r="E112" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B113" t="s">
         <v>210</v>
       </c>
       <c r="C113" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D113" t="s">
         <v>209</v>
       </c>
       <c r="E113" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>210</v>
       </c>
       <c r="C114" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D114" t="s">
         <v>209</v>
       </c>
       <c r="E114" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B115" t="s">
         <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D115" t="s">
         <v>209</v>
       </c>
       <c r="E115" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B116" t="s">
-        <v>275</v>
+        <v>210</v>
       </c>
       <c r="C116" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D116" t="s">
         <v>209</v>
       </c>
       <c r="E116" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B117" t="s">
         <v>210</v>
       </c>
       <c r="C117" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D117" t="s">
         <v>209</v>
       </c>
       <c r="E117" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="C118" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D118" t="s">
         <v>209</v>
       </c>
       <c r="E118" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B119" t="s">
         <v>210</v>
       </c>
       <c r="C119" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D119" t="s">
         <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B120" t="s">
         <v>210</v>
       </c>
       <c r="C120" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D120" t="s">
         <v>209</v>
       </c>
       <c r="E120" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B121" t="s">
         <v>210</v>
       </c>
       <c r="C121" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D121" t="s">
         <v>209</v>
       </c>
       <c r="E121" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B122" t="s">
         <v>210</v>
       </c>
       <c r="C122" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D122" t="s">
         <v>209</v>
       </c>
       <c r="E122" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B123" t="s">
         <v>210</v>
       </c>
       <c r="C123" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
       <c r="D123" t="s">
         <v>209</v>
       </c>
       <c r="E123" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B124" t="s">
         <v>210</v>
       </c>
       <c r="C124" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D124" t="s">
         <v>209</v>
       </c>
       <c r="E124" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B125" t="s">
         <v>210</v>
       </c>
       <c r="C125" t="s">
-        <v>205</v>
+        <v>277</v>
       </c>
       <c r="D125" t="s">
         <v>209</v>
       </c>
       <c r="E125" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B126" t="s">
         <v>210</v>
       </c>
       <c r="C126" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D126" t="s">
         <v>209</v>
       </c>
       <c r="E126" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B127" t="s">
         <v>210</v>
       </c>
       <c r="C127" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D127" t="s">
         <v>209</v>
       </c>
       <c r="E127" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B128" t="s">
         <v>210</v>
       </c>
       <c r="C128" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D128" t="s">
         <v>209</v>
       </c>
       <c r="E128" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="6" t="s">
-        <v>274</v>
+      <c r="A129" t="s">
+        <v>207</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
-      <c r="C129" s="6" t="s">
-        <v>274</v>
+      <c r="C129" t="s">
+        <v>207</v>
       </c>
       <c r="D129" t="s">
         <v>209</v>
       </c>
       <c r="E129" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>208</v>
+      </c>
+      <c r="B130" t="s">
+        <v>210</v>
+      </c>
+      <c r="C130" t="s">
+        <v>208</v>
+      </c>
+      <c r="D130" t="s">
+        <v>209</v>
+      </c>
+      <c r="E130" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B131" t="s">
+        <v>210</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D131" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>278</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
         <v>148</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C132" t="s">
         <v>278</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D132" t="s">
         <v>97</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E132" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>280</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B133" t="s">
         <v>148</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C133" t="s">
         <v>280</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D133" t="s">
         <v>97</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E133" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática: 2025-04-14 08:55:17
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp44351\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2976E6A3-0355-4DDF-B4E2-4A588F81910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30D2FCD-BB4E-419B-9F49-2494B81AA31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2236,7 @@
         <v>282</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>283</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-04-14 08:57:18
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp44351\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30D2FCD-BB4E-419B-9F49-2494B81AA31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615351AB-066B-4EA5-8007-7DAE7F872766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-04-14 09:05:05
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp44351\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615351AB-066B-4EA5-8007-7DAE7F872766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974C6554-AC5A-49FF-A213-00CF895D7E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2230,13 +2230,13 @@
         <v>282</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>282</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>283</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-04-21 08:35:20
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp44351\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\3\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974C6554-AC5A-49FF-A213-00CF895D7E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3266F-DBEE-447F-B9D2-5208457D7B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="284">
   <si>
     <t>Host</t>
   </si>
@@ -1228,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,1535 +1985,1529 @@
       <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>93</v>
+      <c r="E45" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>98</v>
+      <c r="A46" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B46" t="s">
         <v>99</v>
       </c>
-      <c r="C46" t="s">
-        <v>98</v>
+      <c r="C46" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
         <v>99</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
         <v>99</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
         <v>99</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>120</v>
+        <v>282</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>120</v>
+        <v>282</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>121</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>282</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>282</v>
+        <v>122</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>283</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B59" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s">
         <v>150</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B61" t="s">
         <v>150</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B62" t="s">
         <v>150</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B63" t="s">
         <v>150</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B64" t="s">
         <v>150</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>150</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
         <v>150</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D66" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D67" t="s">
         <v>97</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
         <v>146</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
         <v>97</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
         <v>146</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D69" t="s">
         <v>97</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D70" t="s">
         <v>97</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="C71" t="s">
+        <v>152</v>
       </c>
       <c r="D71" t="s">
         <v>97</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>149</v>
+      <c r="E71" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>152</v>
+      <c r="A72" t="s">
+        <v>270</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>270</v>
       </c>
       <c r="D72" t="s">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="E72" t="s">
-        <v>154</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B73" t="s">
         <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D73" t="s">
         <v>209</v>
       </c>
       <c r="E73" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B74" t="s">
         <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D74" t="s">
         <v>209</v>
       </c>
       <c r="E74" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B75" t="s">
         <v>210</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D75" t="s">
         <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>273</v>
+        <v>155</v>
       </c>
       <c r="B76" t="s">
         <v>210</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
+        <v>155</v>
       </c>
       <c r="D76" t="s">
         <v>209</v>
       </c>
       <c r="E76" t="s">
-        <v>269</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
         <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D77" t="s">
         <v>209</v>
       </c>
       <c r="E77" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
         <v>210</v>
       </c>
       <c r="C78" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D78" t="s">
         <v>209</v>
       </c>
       <c r="E78" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B79" t="s">
         <v>210</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D79" t="s">
         <v>209</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
         <v>210</v>
       </c>
       <c r="C80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D80" t="s">
         <v>209</v>
       </c>
       <c r="E80" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
         <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D81" t="s">
         <v>209</v>
       </c>
       <c r="E81" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
         <v>210</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D82" t="s">
         <v>209</v>
       </c>
       <c r="E82" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B83" t="s">
         <v>210</v>
       </c>
       <c r="C83" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D83" t="s">
         <v>209</v>
       </c>
       <c r="E83" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
         <v>210</v>
       </c>
       <c r="C84" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D84" t="s">
         <v>209</v>
       </c>
       <c r="E84" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B85" t="s">
         <v>210</v>
       </c>
       <c r="C85" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D85" t="s">
         <v>209</v>
       </c>
       <c r="E85" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
         <v>210</v>
       </c>
       <c r="C86" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D86" t="s">
         <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
         <v>210</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D87" t="s">
         <v>209</v>
       </c>
       <c r="E87" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
         <v>210</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D88" t="s">
         <v>209</v>
       </c>
       <c r="E88" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
         <v>210</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D89" t="s">
         <v>209</v>
       </c>
       <c r="E89" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
         <v>210</v>
       </c>
       <c r="C90" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D90" t="s">
         <v>209</v>
       </c>
       <c r="E90" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B91" t="s">
         <v>210</v>
       </c>
       <c r="C91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D91" t="s">
         <v>209</v>
       </c>
       <c r="E91" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B92" t="s">
         <v>210</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D92" t="s">
         <v>209</v>
       </c>
       <c r="E92" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B93" t="s">
         <v>210</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D93" t="s">
         <v>209</v>
       </c>
       <c r="E93" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
         <v>210</v>
       </c>
       <c r="C94" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D94" t="s">
         <v>209</v>
       </c>
       <c r="E94" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
         <v>210</v>
       </c>
       <c r="C95" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D95" t="s">
         <v>209</v>
       </c>
       <c r="E95" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
         <v>210</v>
       </c>
       <c r="C96" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D96" t="s">
         <v>209</v>
       </c>
       <c r="E96" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
         <v>210</v>
       </c>
       <c r="C97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D97" t="s">
         <v>209</v>
       </c>
       <c r="E97" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
         <v>210</v>
       </c>
       <c r="C98" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D98" t="s">
         <v>209</v>
       </c>
       <c r="E98" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B99" t="s">
         <v>210</v>
       </c>
       <c r="C99" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D99" t="s">
         <v>209</v>
       </c>
       <c r="E99" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D100" t="s">
         <v>209</v>
       </c>
       <c r="E100" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B101" t="s">
-        <v>276</v>
+        <v>210</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D101" t="s">
         <v>209</v>
       </c>
       <c r="E101" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B102" t="s">
         <v>210</v>
       </c>
       <c r="C102" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D102" t="s">
         <v>209</v>
       </c>
       <c r="E102" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B103" t="s">
         <v>210</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D103" t="s">
         <v>209</v>
       </c>
       <c r="E103" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
         <v>210</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D104" t="s">
         <v>209</v>
       </c>
       <c r="E104" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B105" t="s">
         <v>210</v>
       </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D105" t="s">
         <v>209</v>
       </c>
       <c r="E105" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B106" t="s">
         <v>210</v>
       </c>
       <c r="C106" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D106" t="s">
         <v>209</v>
       </c>
       <c r="E106" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B107" t="s">
         <v>210</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D107" t="s">
         <v>209</v>
       </c>
       <c r="E107" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B108" t="s">
         <v>210</v>
       </c>
       <c r="C108" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D108" t="s">
         <v>209</v>
       </c>
       <c r="E108" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B109" t="s">
         <v>210</v>
       </c>
       <c r="C109" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D109" t="s">
         <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B110" t="s">
         <v>210</v>
       </c>
       <c r="C110" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D110" t="s">
         <v>209</v>
       </c>
       <c r="E110" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
         <v>210</v>
       </c>
       <c r="C111" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D111" t="s">
         <v>209</v>
       </c>
       <c r="E111" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B112" t="s">
         <v>210</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D112" t="s">
         <v>209</v>
       </c>
       <c r="E112" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B113" t="s">
         <v>210</v>
       </c>
       <c r="C113" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D113" t="s">
         <v>209</v>
       </c>
       <c r="E113" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
         <v>210</v>
       </c>
       <c r="C114" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D114" t="s">
         <v>209</v>
       </c>
       <c r="E114" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B115" t="s">
         <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D115" t="s">
         <v>209</v>
       </c>
       <c r="E115" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B116" t="s">
         <v>210</v>
       </c>
       <c r="C116" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D116" t="s">
         <v>209</v>
       </c>
       <c r="E116" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B117" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="C117" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D117" t="s">
         <v>209</v>
       </c>
       <c r="E117" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B118" t="s">
-        <v>275</v>
+        <v>210</v>
       </c>
       <c r="C118" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D118" t="s">
         <v>209</v>
       </c>
       <c r="E118" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B119" t="s">
         <v>210</v>
       </c>
       <c r="C119" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D119" t="s">
         <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B120" t="s">
         <v>210</v>
       </c>
       <c r="C120" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D120" t="s">
         <v>209</v>
       </c>
       <c r="E120" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B121" t="s">
         <v>210</v>
       </c>
       <c r="C121" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D121" t="s">
         <v>209</v>
       </c>
       <c r="E121" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B122" t="s">
         <v>210</v>
       </c>
       <c r="C122" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D122" t="s">
         <v>209</v>
       </c>
       <c r="E122" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B123" t="s">
         <v>210</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D123" t="s">
         <v>209</v>
       </c>
       <c r="E123" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B124" t="s">
         <v>210</v>
       </c>
       <c r="C124" t="s">
-        <v>202</v>
+        <v>277</v>
       </c>
       <c r="D124" t="s">
         <v>209</v>
       </c>
       <c r="E124" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B125" t="s">
         <v>210</v>
       </c>
       <c r="C125" t="s">
-        <v>277</v>
+        <v>204</v>
       </c>
       <c r="D125" t="s">
         <v>209</v>
       </c>
       <c r="E125" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B126" t="s">
         <v>210</v>
       </c>
       <c r="C126" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D126" t="s">
         <v>209</v>
       </c>
       <c r="E126" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B127" t="s">
         <v>210</v>
       </c>
       <c r="C127" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D127" t="s">
         <v>209</v>
       </c>
       <c r="E127" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B128" t="s">
         <v>210</v>
       </c>
       <c r="C128" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D128" t="s">
         <v>209</v>
       </c>
       <c r="E128" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
       </c>
       <c r="C129" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D129" t="s">
         <v>209</v>
       </c>
       <c r="E129" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>208</v>
+      <c r="A130" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="B130" t="s">
         <v>210</v>
       </c>
-      <c r="C130" t="s">
-        <v>208</v>
+      <c r="C130" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="D130" t="s">
         <v>209</v>
       </c>
       <c r="E130" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="6" t="s">
-        <v>274</v>
+      <c r="A131" t="s">
+        <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>210</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>274</v>
+        <v>148</v>
+      </c>
+      <c r="C131" t="s">
+        <v>278</v>
       </c>
       <c r="D131" t="s">
-        <v>209</v>
+        <v>97</v>
       </c>
       <c r="E131" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B132" t="s">
         <v>148</v>
       </c>
       <c r="C132" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D132" t="s">
         <v>97</v>
       </c>
       <c r="E132" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>280</v>
-      </c>
-      <c r="B133" t="s">
-        <v>148</v>
-      </c>
-      <c r="C133" t="s">
-        <v>280</v>
-      </c>
-      <c r="D133" t="s">
-        <v>97</v>
-      </c>
-      <c r="E133" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-09 17:26:55
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\3\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\5\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3266F-DBEE-447F-B9D2-5208457D7B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F70CCF8-442B-481E-9ACE-9633D3F56A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="282">
   <si>
     <t>Host</t>
   </si>
@@ -180,9 +180,6 @@
     <t>10.181.3.79</t>
   </si>
   <si>
-    <t>10.181.4.115</t>
-  </si>
-  <si>
     <t>alkexadbadm01vm2</t>
   </si>
   <si>
@@ -304,9 +301,6 @@
   </si>
   <si>
     <t>DBORACLEIDMAN02</t>
-  </si>
-  <si>
-    <t>ALKANADBBOGDIS</t>
   </si>
   <si>
     <t xml:space="preserve">ANSIBLE </t>
@@ -1228,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1254,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,13 +1262,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -1294,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1328,7 +1322,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,7 +1373,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1396,7 +1390,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,7 +1441,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1464,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,7 +1475,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1515,10 +1509,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1535,10 +1529,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1555,10 +1549,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1575,10 +1569,10 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1595,7 +1589,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,7 +1606,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1629,7 +1623,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1646,7 +1640,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,10 +1657,10 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1700,7 +1694,7 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1717,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1751,7 +1745,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1768,7 +1762,7 @@
         <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,7 +1779,7 @@
         <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1802,7 +1796,7 @@
         <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,7 +1813,7 @@
         <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1836,7 +1830,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1853,7 +1847,7 @@
         <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1870,7 +1864,7 @@
         <v>37</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,7 +1881,7 @@
         <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,7 +1898,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1921,10 +1915,10 @@
         <v>7</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,7 +1935,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1958,10 +1952,10 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1995,35 +1989,35 @@
         <v>7</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>93</v>
+      <c r="E44" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>98</v>
+      <c r="A45" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -2037,7 +2031,7 @@
         <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>101</v>
@@ -2054,7 +2048,7 @@
         <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>103</v>
@@ -2071,7 +2065,7 @@
         <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>105</v>
@@ -2088,7 +2082,7 @@
         <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>107</v>
@@ -2105,7 +2099,7 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>109</v>
@@ -2122,7 +2116,7 @@
         <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>111</v>
@@ -2139,7 +2133,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>113</v>
@@ -2156,7 +2150,7 @@
         <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>115</v>
@@ -2165,24 +2159,24 @@
         <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="B54" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2190,13 +2184,13 @@
         <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>118</v>
       </c>
       <c r="D55" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>119</v>
@@ -2204,36 +2198,36 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>120</v>
+        <v>280</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>120</v>
+        <v>280</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>121</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>282</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>282</v>
+        <v>120</v>
       </c>
       <c r="D57" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>283</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2241,7 +2235,7 @@
         <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>122</v>
@@ -2258,7 +2252,7 @@
         <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>124</v>
@@ -2275,7 +2269,7 @@
         <v>126</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>126</v>
@@ -2292,7 +2286,7 @@
         <v>128</v>
       </c>
       <c r="B61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>128</v>
@@ -2309,7 +2303,7 @@
         <v>130</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>130</v>
@@ -2326,7 +2320,7 @@
         <v>132</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>132</v>
@@ -2343,13 +2337,13 @@
         <v>134</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>135</v>
@@ -2360,13 +2354,13 @@
         <v>136</v>
       </c>
       <c r="B65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>136</v>
       </c>
       <c r="D65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>137</v>
@@ -2377,914 +2371,914 @@
         <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D66" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B69" t="s">
         <v>146</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D69" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>148</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="C70" t="s">
+        <v>150</v>
       </c>
       <c r="D70" t="s">
-        <v>97</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>149</v>
+        <v>95</v>
+      </c>
+      <c r="E70" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>152</v>
+      <c r="A71" t="s">
+        <v>268</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
+        <v>208</v>
       </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>268</v>
       </c>
       <c r="D71" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="E71" t="s">
-        <v>154</v>
+        <v>264</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B72" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E73" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>273</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C75" t="s">
-        <v>273</v>
+        <v>153</v>
       </c>
       <c r="D75" t="s">
+        <v>207</v>
+      </c>
+      <c r="E75" t="s">
         <v>209</v>
-      </c>
-      <c r="E75" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B76" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" t="s">
+        <v>154</v>
+      </c>
+      <c r="D76" t="s">
+        <v>207</v>
+      </c>
+      <c r="E76" t="s">
         <v>210</v>
-      </c>
-      <c r="C76" t="s">
-        <v>155</v>
-      </c>
-      <c r="D76" t="s">
-        <v>209</v>
-      </c>
-      <c r="E76" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D77" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B78" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D79" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D80" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D81" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B82" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D82" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D83" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D84" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D85" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E85" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D86" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E86" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C87" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D87" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D89" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D90" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D91" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B92" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D92" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B93" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D93" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B94" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D94" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D95" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C97" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D97" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C98" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D98" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B99" t="s">
-        <v>210</v>
+        <v>274</v>
       </c>
       <c r="C99" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D99" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B100" t="s">
-        <v>276</v>
+        <v>208</v>
       </c>
       <c r="C100" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D100" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C102" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D102" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C103" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D103" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C104" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D104" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D105" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D106" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C107" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D107" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D108" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B109" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D109" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B110" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D110" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B111" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C111" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D111" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E111" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B112" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C112" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D112" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E112" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C113" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D113" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D114" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C115" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D115" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E115" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B116" t="s">
-        <v>210</v>
+        <v>273</v>
       </c>
       <c r="C116" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D116" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B117" t="s">
-        <v>275</v>
+        <v>208</v>
       </c>
       <c r="C117" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D117" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E117" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C118" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D118" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B119" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C119" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D119" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E119" t="s">
         <v>254</v>
@@ -3292,189 +3286,189 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D120" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B121" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C121" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D121" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E121" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B122" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D122" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B123" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C123" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
       <c r="D123" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E123" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B124" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C124" t="s">
-        <v>277</v>
+        <v>202</v>
       </c>
       <c r="D124" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E124" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B125" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C125" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D125" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E125" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B126" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C126" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D126" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E126" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B127" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C127" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D127" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E127" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B128" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C128" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D128" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E128" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>208</v>
+      <c r="A129" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="B129" t="s">
-        <v>210</v>
-      </c>
-      <c r="C129" t="s">
-        <v>208</v>
+        <v>208</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="D129" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E129" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="6" t="s">
-        <v>274</v>
+      <c r="A130" t="s">
+        <v>276</v>
       </c>
       <c r="B130" t="s">
-        <v>210</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>274</v>
+        <v>146</v>
+      </c>
+      <c r="C130" t="s">
+        <v>276</v>
       </c>
       <c r="D130" t="s">
-        <v>209</v>
+        <v>95</v>
       </c>
       <c r="E130" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,33 +3476,16 @@
         <v>278</v>
       </c>
       <c r="B131" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C131" t="s">
         <v>278</v>
       </c>
       <c r="D131" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E131" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>280</v>
-      </c>
-      <c r="B132" t="s">
-        <v>148</v>
-      </c>
-      <c r="C132" t="s">
-        <v>280</v>
-      </c>
-      <c r="D132" t="s">
-        <v>97</v>
-      </c>
-      <c r="E132" t="s">
-        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-14 15:20:36
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\5\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp03938\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F70CCF8-442B-481E-9ACE-9633D3F56A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64805EE5-6B8B-4D5A-8840-C2641548CD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="285">
   <si>
     <t>Host</t>
   </si>
@@ -871,6 +871,15 @@
   </si>
   <si>
     <t>central-qa3</t>
+  </si>
+  <si>
+    <t>10.206.42.11</t>
+  </si>
+  <si>
+    <t>alka1-n1</t>
+  </si>
+  <si>
+    <t>Srv_Geo_Prd</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,6 +3497,23 @@
         <v>279</v>
       </c>
     </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>282</v>
+      </c>
+      <c r="B132" t="s">
+        <v>284</v>
+      </c>
+      <c r="C132" t="s">
+        <v>282</v>
+      </c>
+      <c r="D132" t="s">
+        <v>207</v>
+      </c>
+      <c r="E132" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-16 15:15:02
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp03938\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp13679\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64805EE5-6B8B-4D5A-8840-C2641548CD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F7890E-DC0A-45BE-99D7-6CF5A99DDC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="287">
   <si>
     <t>Host</t>
   </si>
@@ -880,6 +880,12 @@
   </si>
   <si>
     <t>Srv_Geo_Prd</t>
+  </si>
+  <si>
+    <t>10.181.9.210</t>
+  </si>
+  <si>
+    <t>geointeres</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3514,6 +3520,23 @@
         <v>283</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>285</v>
+      </c>
+      <c r="B133" t="s">
+        <v>284</v>
+      </c>
+      <c r="C133" t="s">
+        <v>285</v>
+      </c>
+      <c r="D133" t="s">
+        <v>95</v>
+      </c>
+      <c r="E133" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-16 15:17:54
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp13679\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F7890E-DC0A-45BE-99D7-6CF5A99DDC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAAA110-EA3A-42B8-BB38-DBA9427BC8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,10 +882,10 @@
     <t>Srv_Geo_Prd</t>
   </si>
   <si>
-    <t>10.181.9.210</t>
-  </si>
-  <si>
     <t>geointeres</t>
+  </si>
+  <si>
+    <t>10.181.8.210</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3522,19 +3522,19 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B133" t="s">
         <v>284</v>
       </c>
       <c r="C133" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D133" t="s">
         <v>95</v>
       </c>
       <c r="E133" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-12 15:03:52
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp13679\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp01547\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAAA110-EA3A-42B8-BB38-DBA9427BC8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C400171-B8EA-4CFE-B6A8-7C8F33F4F8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="289">
   <si>
     <t>Host</t>
   </si>
@@ -886,6 +886,12 @@
   </si>
   <si>
     <t>10.181.8.210</t>
+  </si>
+  <si>
+    <t>10.181.9.80</t>
+  </si>
+  <si>
+    <t>moncajageo</t>
   </si>
 </sst>
 </file>
@@ -1237,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,6 +3543,23 @@
         <v>285</v>
       </c>
     </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>287</v>
+      </c>
+      <c r="B134" t="s">
+        <v>284</v>
+      </c>
+      <c r="C134" t="s">
+        <v>287</v>
+      </c>
+      <c r="D134" t="s">
+        <v>95</v>
+      </c>
+      <c r="E134" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-07-11 11:50:13
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp01547\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp48193\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110BBBE2-6926-45D2-93D4-3C67A624658D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B843D7-6FA0-488D-8BB8-226A5117D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="293">
   <si>
     <t>Host</t>
   </si>
@@ -892,13 +892,25 @@
   </si>
   <si>
     <t>moncajageo</t>
+  </si>
+  <si>
+    <t>10.181.11.55</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tux </t>
+  </si>
+  <si>
+    <t>mantis-qa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -926,6 +938,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -947,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -963,6 +981,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1243,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3560,6 +3579,23 @@
         <v>288</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>289</v>
+      </c>
+      <c r="B135" t="s">
+        <v>290</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D135" t="s">
+        <v>291</v>
+      </c>
+      <c r="E135" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-07-11 12:14:50
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp48193\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\8\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B843D7-6FA0-488D-8BB8-226A5117D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29234DF1-49EA-466E-A432-8984C4DF91C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="292">
   <si>
     <t>Host</t>
   </si>
@@ -898,9 +898,6 @@
   </si>
   <si>
     <t>Mantis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tux </t>
   </si>
   <si>
     <t>mantis-qa</t>
@@ -1265,7 +1262,7 @@
   <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="E140" sqref="E140"/>
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3590,10 +3587,10 @@
         <v>289</v>
       </c>
       <c r="D135" t="s">
+        <v>95</v>
+      </c>
+      <c r="E135" t="s">
         <v>291</v>
-      </c>
-      <c r="E135" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-05 14:41:36
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\8\0\root@10.181.8.209\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp39828\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29234DF1-49EA-466E-A432-8984C4DF91C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8841F610-9C06-4264-92E8-B8506FDF2231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="294">
   <si>
     <t>Host</t>
   </si>
@@ -901,6 +901,12 @@
   </si>
   <si>
     <t>mantis-qa</t>
+  </si>
+  <si>
+    <t>10.181.11.57</t>
+  </si>
+  <si>
+    <t>geopruebasOL10</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3593,6 +3599,23 @@
         <v>291</v>
       </c>
     </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>292</v>
+      </c>
+      <c r="B136" t="s">
+        <v>208</v>
+      </c>
+      <c r="C136" t="s">
+        <v>292</v>
+      </c>
+      <c r="D136" t="s">
+        <v>95</v>
+      </c>
+      <c r="E136" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-15 15:46:26
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp39828\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp43173\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8841F610-9C06-4264-92E8-B8506FDF2231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED3F5A-FE6C-4F2C-A781-DB63A43F11CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="298">
   <si>
     <t>Host</t>
   </si>
@@ -907,6 +907,18 @@
   </si>
   <si>
     <t>geopruebasOL10</t>
+  </si>
+  <si>
+    <t>10.181.11.117</t>
+  </si>
+  <si>
+    <t>Srv_gestionIP</t>
+  </si>
+  <si>
+    <t>10.181.11.227</t>
+  </si>
+  <si>
+    <t>gestionips</t>
   </si>
 </sst>
 </file>
@@ -1265,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3616,6 +3628,23 @@
         <v>293</v>
       </c>
     </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>294</v>
+      </c>
+      <c r="B137" t="s">
+        <v>295</v>
+      </c>
+      <c r="C137" t="s">
+        <v>296</v>
+      </c>
+      <c r="D137" t="s">
+        <v>95</v>
+      </c>
+      <c r="E137" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-15 15:55:30
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp43173\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED3F5A-FE6C-4F2C-A781-DB63A43F11CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E0646-E946-411E-B39B-9841B1FBB115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="297">
   <si>
     <t>Host</t>
   </si>
@@ -907,9 +907,6 @@
   </si>
   <si>
     <t>geopruebasOL10</t>
-  </si>
-  <si>
-    <t>10.181.11.117</t>
   </si>
   <si>
     <t>Srv_gestionIP</t>
@@ -1279,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,19 +3627,19 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>295</v>
+      </c>
+      <c r="B137" t="s">
         <v>294</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>295</v>
-      </c>
-      <c r="C137" t="s">
-        <v>296</v>
       </c>
       <c r="D137" t="s">
         <v>95</v>
       </c>
       <c r="E137" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-27 08:55:25
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp43173\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp52136\ansible\Inventory\dynamic_inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E0646-E946-411E-B39B-9841B1FBB115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33315AD6-DE27-467B-8AEA-D1BDE92D73B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="300">
   <si>
     <t>Host</t>
   </si>
@@ -916,6 +916,15 @@
   </si>
   <si>
     <t>gestionips</t>
+  </si>
+  <si>
+    <t>PlantGeoOL9</t>
+  </si>
+  <si>
+    <t>10.181.11.58</t>
+  </si>
+  <si>
+    <t>geopruebasOL9</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,6 +3651,23 @@
         <v>296</v>
       </c>
     </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>298</v>
+      </c>
+      <c r="B138" t="s">
+        <v>297</v>
+      </c>
+      <c r="C138" t="s">
+        <v>298</v>
+      </c>
+      <c r="D138" t="s">
+        <v>95</v>
+      </c>
+      <c r="E138" t="s">
+        <v>299</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-09-03 09:44:52
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7167351\AppData\Local\Temp\scp52136\ansible\Inventory\dynamic_inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\102627~1\AppData\Roaming\MobaXterm\slash\FTPRemoteFiles\3\0\root@10.181.8.209\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33315AD6-DE27-467B-8AEA-D1BDE92D73B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935998A-7AC4-4542-8FE5-2F8AB7340EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="303">
   <si>
     <t>Host</t>
   </si>
@@ -925,6 +925,15 @@
   </si>
   <si>
     <t>geopruebasOL9</t>
+  </si>
+  <si>
+    <t>10.181.8.218</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>POC pruebas</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3668,6 +3677,23 @@
         <v>299</v>
       </c>
     </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>300</v>
+      </c>
+      <c r="B139" t="s">
+        <v>301</v>
+      </c>
+      <c r="C139" t="s">
+        <v>300</v>
+      </c>
+      <c r="D139" t="s">
+        <v>95</v>
+      </c>
+      <c r="E139" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>